<commit_message>
#Fix bug: 128613, Change #128615
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -1370,7 +1370,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1529,9 +1529,6 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1569,14 +1566,20 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -3210,17 +3213,17 @@
       <c r="GF8" s="47"/>
     </row>
     <row r="9" spans="1:188" s="43" customFormat="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
-      <c r="K9" s="56"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
+      <c r="K9" s="55"/>
       <c r="L9" s="45" t="s">
         <v>10</v>
       </c>
@@ -3274,7 +3277,7 @@
       <c r="AN9" s="48"/>
       <c r="AO9" s="48"/>
       <c r="AP9" s="53"/>
-      <c r="AQ9" s="54" t="s">
+      <c r="AQ9" s="69" t="s">
         <v>33</v>
       </c>
       <c r="AR9" s="49" t="s">
@@ -3367,16 +3370,16 @@
         <v>60</v>
       </c>
       <c r="CY9" s="47"/>
-      <c r="CZ9" s="55"/>
-      <c r="DA9" s="56"/>
-      <c r="DB9" s="56"/>
-      <c r="DC9" s="56"/>
-      <c r="DD9" s="56"/>
-      <c r="DE9" s="56"/>
-      <c r="DF9" s="57"/>
-      <c r="DG9" s="58"/>
-      <c r="DH9" s="59"/>
-      <c r="DI9" s="60"/>
+      <c r="CZ9" s="54"/>
+      <c r="DA9" s="55"/>
+      <c r="DB9" s="55"/>
+      <c r="DC9" s="55"/>
+      <c r="DD9" s="55"/>
+      <c r="DE9" s="55"/>
+      <c r="DF9" s="56"/>
+      <c r="DG9" s="57"/>
+      <c r="DH9" s="58"/>
+      <c r="DI9" s="59"/>
       <c r="DJ9" s="45" t="s">
         <v>68</v>
       </c>
@@ -3426,7 +3429,7 @@
       <c r="ER9" s="46"/>
       <c r="ES9" s="46"/>
       <c r="ET9" s="47"/>
-      <c r="EU9" s="61" t="s">
+      <c r="EU9" s="60" t="s">
         <v>86</v>
       </c>
       <c r="EV9" s="51" t="s">
@@ -3439,8 +3442,8 @@
       <c r="EY9" s="46"/>
       <c r="EZ9" s="46"/>
       <c r="FA9" s="47"/>
-      <c r="FB9" s="55"/>
-      <c r="FC9" s="57"/>
+      <c r="FB9" s="54"/>
+      <c r="FC9" s="56"/>
       <c r="FD9" s="45" t="s">
         <v>151</v>
       </c>
@@ -3453,14 +3456,14 @@
       <c r="FK9" s="46"/>
       <c r="FL9" s="46"/>
       <c r="FM9" s="47"/>
-      <c r="FN9" s="62"/>
-      <c r="FO9" s="57"/>
-      <c r="FP9" s="62"/>
-      <c r="FQ9" s="57"/>
-      <c r="FR9" s="55"/>
-      <c r="FS9" s="57"/>
-      <c r="FT9" s="55"/>
-      <c r="FU9" s="56"/>
+      <c r="FN9" s="61"/>
+      <c r="FO9" s="56"/>
+      <c r="FP9" s="61"/>
+      <c r="FQ9" s="56"/>
+      <c r="FR9" s="54"/>
+      <c r="FS9" s="56"/>
+      <c r="FT9" s="54"/>
+      <c r="FU9" s="55"/>
       <c r="FV9" s="45" t="s">
         <v>114</v>
       </c>
@@ -3469,573 +3472,573 @@
         <v>115</v>
       </c>
       <c r="FY9" s="47"/>
-      <c r="FZ9" s="63"/>
-      <c r="GA9" s="55"/>
-      <c r="GB9" s="64" t="s">
+      <c r="FZ9" s="62"/>
+      <c r="GA9" s="54"/>
+      <c r="GB9" s="71" t="s">
         <v>120</v>
       </c>
       <c r="GC9" s="47"/>
-      <c r="GD9" s="64" t="s">
+      <c r="GD9" s="71" t="s">
         <v>174</v>
       </c>
       <c r="GE9" s="46"/>
       <c r="GF9" s="47"/>
     </row>
     <row r="10" spans="1:188" s="43" customFormat="1" ht="12" customHeight="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="65" t="s">
         <v>162</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="J10" s="66" t="s">
+      <c r="J10" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="K10" s="66" t="s">
+      <c r="K10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="M10" s="67" t="s">
+      <c r="M10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="N10" s="67" t="s">
+      <c r="N10" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="O10" s="67" t="s">
+      <c r="O10" s="66" t="s">
         <v>160</v>
       </c>
-      <c r="P10" s="67" t="s">
+      <c r="P10" s="66" t="s">
         <v>161</v>
       </c>
-      <c r="Q10" s="67" t="s">
+      <c r="Q10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="S10" s="67" t="s">
+      <c r="S10" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="T10" s="67"/>
-      <c r="U10" s="67" t="s">
+      <c r="T10" s="66"/>
+      <c r="U10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="V10" s="67" t="s">
+      <c r="V10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="W10" s="67" t="s">
+      <c r="W10" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="X10" s="67" t="s">
+      <c r="X10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="Y10" s="67" t="s">
+      <c r="Y10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="Z10" s="67" t="s">
+      <c r="Z10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AA10" s="67" t="s">
+      <c r="AA10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="AB10" s="67" t="s">
+      <c r="AB10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AC10" s="67" t="s">
+      <c r="AC10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AD10" s="67" t="s">
+      <c r="AD10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="AE10" s="67" t="s">
+      <c r="AE10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AF10" s="67" t="s">
+      <c r="AF10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AG10" s="67" t="s">
+      <c r="AG10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AH10" s="67" t="s">
+      <c r="AH10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AI10" s="67" t="s">
+      <c r="AI10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AJ10" s="67" t="s">
+      <c r="AJ10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AK10" s="67" t="s">
+      <c r="AK10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AL10" s="67" t="s">
+      <c r="AL10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AM10" s="67" t="s">
+      <c r="AM10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AN10" s="67" t="s">
+      <c r="AN10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AO10" s="67" t="s">
+      <c r="AO10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AP10" s="67" t="s">
+      <c r="AP10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AQ10" s="68"/>
-      <c r="AR10" s="67" t="s">
+      <c r="AQ10" s="70"/>
+      <c r="AR10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AS10" s="67" t="s">
+      <c r="AS10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AT10" s="67" t="s">
+      <c r="AT10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AU10" s="67" t="s">
+      <c r="AU10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AV10" s="67" t="s">
+      <c r="AV10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="AW10" s="67" t="s">
+      <c r="AW10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AX10" s="67" t="s">
+      <c r="AX10" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="AY10" s="67" t="s">
+      <c r="AY10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="AZ10" s="67" t="s">
+      <c r="AZ10" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="BA10" s="67" t="s">
+      <c r="BA10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="BB10" s="67" t="s">
+      <c r="BB10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="BC10" s="67" t="s">
+      <c r="BC10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="BD10" s="67" t="s">
+      <c r="BD10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="BE10" s="67" t="s">
+      <c r="BE10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="BF10" s="67" t="s">
+      <c r="BF10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BG10" s="67" t="s">
+      <c r="BG10" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="BH10" s="67" t="s">
+      <c r="BH10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="BI10" s="67" t="s">
+      <c r="BI10" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="BJ10" s="67" t="s">
+      <c r="BJ10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="BK10" s="67" t="s">
+      <c r="BK10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="BL10" s="67" t="s">
+      <c r="BL10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="BM10" s="67" t="s">
+      <c r="BM10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="BN10" s="67" t="s">
+      <c r="BN10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="BO10" s="67" t="s">
+      <c r="BO10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BP10" s="67" t="s">
+      <c r="BP10" s="66" t="s">
         <v>163</v>
       </c>
-      <c r="BQ10" s="67" t="s">
+      <c r="BQ10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="BR10" s="67" t="s">
+      <c r="BR10" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="BS10" s="67" t="s">
+      <c r="BS10" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="BT10" s="67" t="s">
+      <c r="BT10" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="BU10" s="67" t="s">
+      <c r="BU10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="BV10" s="67" t="s">
+      <c r="BV10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="BW10" s="67" t="s">
+      <c r="BW10" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="BX10" s="67" t="s">
+      <c r="BX10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="BY10" s="67" t="s">
+      <c r="BY10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="BZ10" s="67" t="s">
+      <c r="BZ10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="CA10" s="67" t="s">
+      <c r="CA10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="CB10" s="67" t="s">
+      <c r="CB10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="CC10" s="67" t="s">
+      <c r="CC10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="CD10" s="67" t="s">
+      <c r="CD10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="CE10" s="67" t="s">
+      <c r="CE10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="CF10" s="67" t="s">
+      <c r="CF10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="CG10" s="67" t="s">
+      <c r="CG10" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="CH10" s="67" t="s">
+      <c r="CH10" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="CI10" s="67" t="s">
+      <c r="CI10" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="CJ10" s="67" t="s">
+      <c r="CJ10" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="CK10" s="67" t="s">
+      <c r="CK10" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="CL10" s="67" t="s">
+      <c r="CL10" s="66" t="s">
         <v>149</v>
       </c>
-      <c r="CM10" s="67" t="s">
+      <c r="CM10" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="CN10" s="67" t="s">
+      <c r="CN10" s="66" t="s">
         <v>150</v>
       </c>
-      <c r="CO10" s="67" t="s">
+      <c r="CO10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CP10" s="67" t="s">
+      <c r="CP10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CQ10" s="67" t="s">
+      <c r="CQ10" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="CR10" s="67" t="s">
+      <c r="CR10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CS10" s="67" t="s">
+      <c r="CS10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CT10" s="67" t="s">
+      <c r="CT10" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="CU10" s="67" t="s">
+      <c r="CU10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CV10" s="67" t="s">
+      <c r="CV10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CW10" s="67" t="s">
+      <c r="CW10" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="CX10" s="67" t="s">
+      <c r="CX10" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="CY10" s="67" t="s">
+      <c r="CY10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="CZ10" s="67" t="s">
+      <c r="CZ10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="DA10" s="67" t="s">
+      <c r="DA10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="DB10" s="67" t="s">
+      <c r="DB10" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="DC10" s="67" t="s">
+      <c r="DC10" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="DD10" s="67" t="s">
+      <c r="DD10" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="DE10" s="67" t="s">
+      <c r="DE10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="DF10" s="67" t="s">
+      <c r="DF10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="DG10" s="67" t="s">
+      <c r="DG10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="DH10" s="67" t="s">
+      <c r="DH10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="DI10" s="67" t="s">
+      <c r="DI10" s="66" t="s">
         <v>164</v>
       </c>
-      <c r="DJ10" s="67" t="s">
+      <c r="DJ10" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="DK10" s="67" t="s">
+      <c r="DK10" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="DL10" s="67" t="s">
+      <c r="DL10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="DM10" s="67" t="s">
+      <c r="DM10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DN10" s="67" t="s">
+      <c r="DN10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DO10" s="67" t="s">
+      <c r="DO10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="DP10" s="67" t="s">
+      <c r="DP10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DQ10" s="67" t="s">
+      <c r="DQ10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DR10" s="67" t="s">
+      <c r="DR10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="DS10" s="67" t="s">
+      <c r="DS10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DT10" s="67" t="s">
+      <c r="DT10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DU10" s="67" t="s">
+      <c r="DU10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="DV10" s="67" t="s">
+      <c r="DV10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DW10" s="67" t="s">
+      <c r="DW10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DX10" s="67" t="s">
+      <c r="DX10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="DY10" s="67" t="s">
+      <c r="DY10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DZ10" s="67" t="s">
+      <c r="DZ10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EA10" s="67" t="s">
+      <c r="EA10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="EB10" s="67" t="s">
+      <c r="EB10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EC10" s="67" t="s">
+      <c r="EC10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="ED10" s="67" t="s">
+      <c r="ED10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="EE10" s="67" t="s">
+      <c r="EE10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EF10" s="67" t="s">
+      <c r="EF10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EG10" s="67" t="s">
+      <c r="EG10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="EH10" s="67" t="s">
+      <c r="EH10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EI10" s="67" t="s">
+      <c r="EI10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EJ10" s="67" t="s">
+      <c r="EJ10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="EK10" s="67" t="s">
+      <c r="EK10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EL10" s="67" t="s">
+      <c r="EL10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EM10" s="67" t="s">
+      <c r="EM10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="EN10" s="67" t="s">
+      <c r="EN10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="EO10" s="67" t="s">
+      <c r="EO10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="EP10" s="67" t="s">
+      <c r="EP10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="EQ10" s="67" t="s">
+      <c r="EQ10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="ER10" s="67" t="s">
+      <c r="ER10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="ES10" s="67" t="s">
+      <c r="ES10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="ET10" s="67" t="s">
+      <c r="ET10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="EU10" s="67" t="s">
+      <c r="EU10" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="EV10" s="67" t="s">
+      <c r="EV10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="EW10" s="67" t="s">
+      <c r="EW10" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="EX10" s="67" t="s">
+      <c r="EX10" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="EY10" s="67" t="s">
+      <c r="EY10" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="EZ10" s="67" t="s">
+      <c r="EZ10" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="FA10" s="67" t="s">
+      <c r="FA10" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="FB10" s="67" t="s">
+      <c r="FB10" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="FC10" s="67" t="s">
+      <c r="FC10" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="FD10" s="67" t="s">
+      <c r="FD10" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="FE10" s="67" t="s">
+      <c r="FE10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="FF10" s="67" t="s">
+      <c r="FF10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="FG10" s="67" t="s">
+      <c r="FG10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="FH10" s="67" t="s">
+      <c r="FH10" s="66" t="s">
         <v>103</v>
       </c>
       <c r="FI10" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="FJ10" s="67" t="s">
+      <c r="FJ10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="FK10" s="67" t="s">
+      <c r="FK10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="FL10" s="67" t="s">
+      <c r="FL10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="FM10" s="67" t="s">
+      <c r="FM10" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="FN10" s="66" t="s">
+      <c r="FN10" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="FO10" s="66" t="s">
+      <c r="FO10" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="FP10" s="66" t="s">
+      <c r="FP10" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="FQ10" s="66" t="s">
+      <c r="FQ10" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="FR10" s="67" t="s">
+      <c r="FR10" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="FS10" s="67" t="s">
+      <c r="FS10" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="FT10" s="67" t="s">
+      <c r="FT10" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="FU10" s="67" t="s">
+      <c r="FU10" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="FV10" s="67" t="s">
+      <c r="FV10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="FW10" s="67" t="s">
+      <c r="FW10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="FX10" s="67" t="s">
+      <c r="FX10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="FY10" s="67" t="s">
+      <c r="FY10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="FZ10" s="66" t="s">
+      <c r="FZ10" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="GA10" s="67" t="s">
+      <c r="GA10" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="GB10" s="69"/>
-      <c r="GC10" s="67" t="s">
+      <c r="GB10" s="72"/>
+      <c r="GC10" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="GD10" s="69"/>
-      <c r="GE10" s="67" t="s">
+      <c r="GD10" s="72"/>
+      <c r="GE10" s="66" t="s">
         <v>122</v>
       </c>
-      <c r="GF10" s="67" t="s">
+      <c r="GF10" s="66" t="s">
         <v>123</v>
       </c>
     </row>
@@ -5969,10 +5972,16 @@
     <col min="32" max="33" width="10.625" style="29"/>
     <col min="34" max="36" width="10.625" style="11"/>
     <col min="37" max="37" width="10.625" style="29"/>
-    <col min="38" max="43" width="10.625" style="11"/>
+    <col min="38" max="39" width="10.625" style="11"/>
+    <col min="40" max="40" width="10.625" style="29"/>
+    <col min="41" max="41" width="10.625" style="11"/>
+    <col min="42" max="42" width="10.625" style="29"/>
+    <col min="43" max="43" width="10.625" style="11"/>
     <col min="44" max="48" width="10.625" style="29"/>
     <col min="49" max="52" width="10.625" style="11"/>
-    <col min="53" max="55" width="10.625" style="29"/>
+    <col min="53" max="53" width="10.625" style="29"/>
+    <col min="54" max="54" width="10.625" style="11"/>
+    <col min="55" max="55" width="10.625" style="29"/>
     <col min="56" max="57" width="10.625" style="11"/>
     <col min="58" max="61" width="10.625" style="29"/>
     <col min="62" max="63" width="10.625" style="11"/>
@@ -6065,7 +6074,6 @@
       <c r="AU1" s="27"/>
       <c r="AV1" s="27"/>
       <c r="BA1" s="27"/>
-      <c r="BB1" s="27"/>
       <c r="BC1" s="27"/>
       <c r="BF1" s="27"/>
       <c r="BG1" s="27"/>
@@ -6145,7 +6153,6 @@
       <c r="AU2" s="27"/>
       <c r="AV2" s="27"/>
       <c r="BA2" s="27"/>
-      <c r="BB2" s="27"/>
       <c r="BC2" s="27"/>
       <c r="BF2" s="27"/>
       <c r="BG2" s="27"/>
@@ -6225,7 +6232,6 @@
       <c r="AU3" s="27"/>
       <c r="AV3" s="27"/>
       <c r="BA3" s="27"/>
-      <c r="BB3" s="27"/>
       <c r="BC3" s="27"/>
       <c r="BF3" s="27"/>
       <c r="BG3" s="27"/>
@@ -6305,7 +6311,6 @@
       <c r="AU4" s="27"/>
       <c r="AV4" s="27"/>
       <c r="BA4" s="27"/>
-      <c r="BB4" s="27"/>
       <c r="BC4" s="27"/>
       <c r="BF4" s="27"/>
       <c r="BG4" s="27"/>
@@ -6363,7 +6368,6 @@
       <c r="AU5" s="27"/>
       <c r="AV5" s="27"/>
       <c r="BA5" s="27"/>
-      <c r="BB5" s="27"/>
       <c r="BC5" s="27"/>
       <c r="BF5" s="27"/>
       <c r="BG5" s="27"/>
@@ -6450,7 +6454,7 @@
       <c r="AY6" s="33"/>
       <c r="AZ6" s="33"/>
       <c r="BA6" s="28"/>
-      <c r="BB6" s="28"/>
+      <c r="BB6" s="33"/>
       <c r="BC6" s="28"/>
       <c r="BD6" s="33"/>
       <c r="BE6" s="33"/>
@@ -6581,7 +6585,6 @@
       <c r="AU7" s="32"/>
       <c r="AV7" s="32"/>
       <c r="BA7" s="32"/>
-      <c r="BB7" s="32"/>
       <c r="BC7" s="32"/>
       <c r="BF7" s="32"/>
       <c r="BG7" s="32"/>
@@ -6806,16 +6809,16 @@
       </c>
     </row>
     <row r="9" spans="1:154" s="43" customFormat="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
       <c r="K9" s="45" t="s">
         <v>10</v>
       </c>
@@ -6851,23 +6854,23 @@
         <v>124</v>
       </c>
       <c r="AC9" s="46"/>
-      <c r="AD9" s="54" t="s">
+      <c r="AD9" s="69" t="s">
         <v>130</v>
       </c>
-      <c r="AE9" s="54" t="s">
+      <c r="AE9" s="69" t="s">
         <v>131</v>
       </c>
-      <c r="AF9" s="55"/>
-      <c r="AG9" s="56"/>
-      <c r="AH9" s="56"/>
-      <c r="AI9" s="56"/>
-      <c r="AJ9" s="56"/>
-      <c r="AK9" s="57"/>
+      <c r="AF9" s="54"/>
+      <c r="AG9" s="55"/>
+      <c r="AH9" s="55"/>
+      <c r="AI9" s="55"/>
+      <c r="AJ9" s="55"/>
+      <c r="AK9" s="56"/>
       <c r="AL9" s="45" t="s">
         <v>169</v>
       </c>
       <c r="AM9" s="47"/>
-      <c r="AN9" s="45" t="s">
+      <c r="AN9" s="63" t="s">
         <v>43</v>
       </c>
       <c r="AO9" s="46"/>
@@ -6894,7 +6897,7 @@
       <c r="BB9" s="46"/>
       <c r="BC9" s="46"/>
       <c r="BD9" s="47"/>
-      <c r="BE9" s="55"/>
+      <c r="BE9" s="54"/>
       <c r="BF9" s="45" t="s">
         <v>179</v>
       </c>
@@ -6922,13 +6925,13 @@
       <c r="BT9" s="46"/>
       <c r="BU9" s="46"/>
       <c r="BV9" s="47"/>
-      <c r="BW9" s="55"/>
-      <c r="BX9" s="56"/>
-      <c r="BY9" s="56"/>
-      <c r="BZ9" s="56"/>
-      <c r="CA9" s="56"/>
-      <c r="CB9" s="56"/>
-      <c r="CC9" s="55"/>
+      <c r="BW9" s="54"/>
+      <c r="BX9" s="55"/>
+      <c r="BY9" s="55"/>
+      <c r="BZ9" s="55"/>
+      <c r="CA9" s="55"/>
+      <c r="CB9" s="55"/>
+      <c r="CC9" s="54"/>
       <c r="CD9" s="45" t="s">
         <v>181</v>
       </c>
@@ -6996,8 +6999,8 @@
       <c r="DV9" s="46"/>
       <c r="DW9" s="46"/>
       <c r="DX9" s="47"/>
-      <c r="DY9" s="55"/>
-      <c r="DZ9" s="57"/>
+      <c r="DY9" s="54"/>
+      <c r="DZ9" s="56"/>
       <c r="EA9" s="49" t="s">
         <v>151</v>
       </c>
@@ -7010,14 +7013,14 @@
       <c r="EH9" s="48"/>
       <c r="EI9" s="48"/>
       <c r="EJ9" s="53"/>
-      <c r="EK9" s="62"/>
-      <c r="EL9" s="57"/>
-      <c r="EM9" s="62"/>
-      <c r="EN9" s="57"/>
-      <c r="EO9" s="55"/>
-      <c r="EP9" s="57"/>
-      <c r="EQ9" s="55"/>
-      <c r="ER9" s="56"/>
+      <c r="EK9" s="61"/>
+      <c r="EL9" s="56"/>
+      <c r="EM9" s="61"/>
+      <c r="EN9" s="56"/>
+      <c r="EO9" s="54"/>
+      <c r="EP9" s="56"/>
+      <c r="EQ9" s="54"/>
+      <c r="ER9" s="55"/>
       <c r="ES9" s="45" t="s">
         <v>114</v>
       </c>
@@ -7026,464 +7029,464 @@
         <v>115</v>
       </c>
       <c r="EV9" s="47"/>
-      <c r="EW9" s="63"/>
-      <c r="EX9" s="71"/>
+      <c r="EW9" s="62"/>
+      <c r="EX9" s="68"/>
     </row>
     <row r="10" spans="1:154" s="43" customFormat="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="65" t="s">
         <v>6</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="66" t="s">
+      <c r="J10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="67" t="s">
+      <c r="K10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="67" t="s">
+      <c r="M10" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="67" t="s">
+      <c r="N10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="O10" s="67" t="s">
+      <c r="O10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="67" t="s">
+      <c r="P10" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="67"/>
-      <c r="R10" s="67" t="s">
+      <c r="Q10" s="66"/>
+      <c r="R10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="67" t="s">
+      <c r="S10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="67" t="s">
+      <c r="T10" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="U10" s="67" t="s">
+      <c r="U10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="V10" s="67" t="s">
+      <c r="V10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="W10" s="67" t="s">
+      <c r="W10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="X10" s="67" t="s">
+      <c r="X10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="Y10" s="67" t="s">
+      <c r="Y10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="Z10" s="67" t="s">
+      <c r="Z10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AA10" s="67" t="s">
+      <c r="AA10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="AB10" s="67" t="s">
+      <c r="AB10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AC10" s="67" t="s">
+      <c r="AC10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AD10" s="68"/>
-      <c r="AE10" s="68"/>
-      <c r="AF10" s="67" t="s">
+      <c r="AD10" s="70"/>
+      <c r="AE10" s="70"/>
+      <c r="AF10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="AG10" s="67" t="s">
+      <c r="AG10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AH10" s="67" t="s">
+      <c r="AH10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AI10" s="67" t="s">
+      <c r="AI10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="AJ10" s="67" t="s">
+      <c r="AJ10" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="AK10" s="67" t="s">
+      <c r="AK10" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="AL10" s="67" t="s">
+      <c r="AL10" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="AM10" s="67" t="s">
+      <c r="AM10" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="AN10" s="67" t="s">
+      <c r="AN10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="AO10" s="67" t="s">
+      <c r="AO10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="AP10" s="67" t="s">
+      <c r="AP10" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="AQ10" s="67" t="s">
+      <c r="AQ10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="AR10" s="67" t="s">
+      <c r="AR10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="AS10" s="67" t="s">
+      <c r="AS10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="AT10" s="67" t="s">
+      <c r="AT10" s="66" t="s">
         <v>134</v>
       </c>
-      <c r="AU10" s="67" t="s">
+      <c r="AU10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="AV10" s="67" t="s">
+      <c r="AV10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="AW10" s="67" t="s">
+      <c r="AW10" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="AX10" s="67" t="s">
+      <c r="AX10" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="AY10" s="67" t="s">
+      <c r="AY10" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="AZ10" s="67" t="s">
+      <c r="AZ10" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="BA10" s="67" t="s">
+      <c r="BA10" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="BB10" s="67" t="s">
+      <c r="BB10" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="BC10" s="67" t="s">
+      <c r="BC10" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="BD10" s="67" t="s">
+      <c r="BD10" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="BE10" s="66" t="s">
+      <c r="BE10" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="BF10" s="67" t="s">
+      <c r="BF10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="BG10" s="67" t="s">
+      <c r="BG10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="BH10" s="67" t="s">
+      <c r="BH10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="BI10" s="67" t="s">
+      <c r="BI10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="BJ10" s="67" t="s">
+      <c r="BJ10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="BK10" s="66" t="s">
+      <c r="BK10" s="65" t="s">
         <v>136</v>
       </c>
-      <c r="BL10" s="67" t="s">
+      <c r="BL10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="BM10" s="67" t="s">
+      <c r="BM10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="BN10" s="67" t="s">
+      <c r="BN10" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="BO10" s="67" t="s">
+      <c r="BO10" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="BP10" s="67" t="s">
+      <c r="BP10" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="BQ10" s="67" t="s">
+      <c r="BQ10" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="BR10" s="67" t="s">
+      <c r="BR10" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="BS10" s="67" t="s">
+      <c r="BS10" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="BT10" s="67" t="s">
+      <c r="BT10" s="66" t="s">
         <v>141</v>
       </c>
-      <c r="BU10" s="67" t="s">
+      <c r="BU10" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="BV10" s="67" t="s">
+      <c r="BV10" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="BW10" s="67" t="s">
+      <c r="BW10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="BX10" s="67" t="s">
+      <c r="BX10" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="BY10" s="67" t="s">
+      <c r="BY10" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="BZ10" s="67" t="s">
+      <c r="BZ10" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="CA10" s="67" t="s">
+      <c r="CA10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="CB10" s="67" t="s">
+      <c r="CB10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="CC10" s="67" t="s">
+      <c r="CC10" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="CD10" s="67" t="s">
+      <c r="CD10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CE10" s="67" t="s">
+      <c r="CE10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CF10" s="67" t="s">
+      <c r="CF10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="CG10" s="67" t="s">
+      <c r="CG10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="CH10" s="67" t="s">
+      <c r="CH10" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="CI10" s="67" t="s">
+      <c r="CI10" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="CJ10" s="67" t="s">
+      <c r="CJ10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="CK10" s="67" t="s">
+      <c r="CK10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="CL10" s="67" t="s">
+      <c r="CL10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="CM10" s="67" t="s">
+      <c r="CM10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="CN10" s="67" t="s">
+      <c r="CN10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="CO10" s="67" t="s">
+      <c r="CO10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="CP10" s="67" t="s">
+      <c r="CP10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="CQ10" s="67" t="s">
+      <c r="CQ10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="CR10" s="67" t="s">
+      <c r="CR10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="CS10" s="67" t="s">
+      <c r="CS10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="CT10" s="67" t="s">
+      <c r="CT10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="CU10" s="67" t="s">
+      <c r="CU10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="CV10" s="67" t="s">
+      <c r="CV10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="CW10" s="67" t="s">
+      <c r="CW10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="CX10" s="67" t="s">
+      <c r="CX10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="CY10" s="67" t="s">
+      <c r="CY10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="CZ10" s="67" t="s">
+      <c r="CZ10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DA10" s="67" t="s">
+      <c r="DA10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DB10" s="67" t="s">
+      <c r="DB10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="DC10" s="67" t="s">
+      <c r="DC10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DD10" s="67" t="s">
+      <c r="DD10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DE10" s="67" t="s">
+      <c r="DE10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="DF10" s="67" t="s">
+      <c r="DF10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DG10" s="67" t="s">
+      <c r="DG10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DH10" s="67" t="s">
+      <c r="DH10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="DI10" s="67" t="s">
+      <c r="DI10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DJ10" s="67" t="s">
+      <c r="DJ10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DK10" s="67" t="s">
+      <c r="DK10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="DL10" s="67" t="s">
+      <c r="DL10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="DM10" s="67" t="s">
+      <c r="DM10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="DN10" s="67" t="s">
+      <c r="DN10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="DO10" s="67" t="s">
+      <c r="DO10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="DP10" s="67" t="s">
+      <c r="DP10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="DQ10" s="67" t="s">
+      <c r="DQ10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="DR10" s="67" t="s">
+      <c r="DR10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="DS10" s="67" t="s">
+      <c r="DS10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="DT10" s="67" t="s">
+      <c r="DT10" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="DU10" s="67" t="s">
+      <c r="DU10" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="DV10" s="67" t="s">
+      <c r="DV10" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="DW10" s="67" t="s">
+      <c r="DW10" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="DX10" s="67" t="s">
+      <c r="DX10" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="DY10" s="67" t="s">
+      <c r="DY10" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="DZ10" s="67" t="s">
+      <c r="DZ10" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="EA10" s="67" t="s">
+      <c r="EA10" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="EB10" s="67" t="s">
+      <c r="EB10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="EC10" s="67" t="s">
+      <c r="EC10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="ED10" s="67" t="s">
+      <c r="ED10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="EE10" s="67" t="s">
+      <c r="EE10" s="66" t="s">
         <v>103</v>
       </c>
       <c r="EF10" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="EG10" s="67" t="s">
+      <c r="EG10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="EH10" s="67" t="s">
+      <c r="EH10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="EI10" s="67" t="s">
+      <c r="EI10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="EJ10" s="67" t="s">
+      <c r="EJ10" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="EK10" s="66" t="s">
+      <c r="EK10" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="EL10" s="66" t="s">
+      <c r="EL10" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="EM10" s="66" t="s">
+      <c r="EM10" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="EN10" s="66" t="s">
+      <c r="EN10" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="EO10" s="67" t="s">
+      <c r="EO10" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="EP10" s="67" t="s">
+      <c r="EP10" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="EQ10" s="67" t="s">
+      <c r="EQ10" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="ER10" s="67" t="s">
+      <c r="ER10" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="ES10" s="67" t="s">
+      <c r="ES10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="ET10" s="67" t="s">
+      <c r="ET10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="EU10" s="67" t="s">
+      <c r="EU10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="EV10" s="67" t="s">
+      <c r="EV10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="EW10" s="66" t="s">
+      <c r="EW10" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="EX10" s="67" t="s">
+      <c r="EX10" s="66" t="s">
         <v>119</v>
       </c>
     </row>
@@ -7527,9 +7530,9 @@
       <c r="AK11" s="16"/>
       <c r="AL11" s="4"/>
       <c r="AM11" s="4"/>
-      <c r="AN11" s="4"/>
+      <c r="AN11" s="15"/>
       <c r="AO11" s="4"/>
-      <c r="AP11" s="4"/>
+      <c r="AP11" s="15"/>
       <c r="AQ11" s="4"/>
       <c r="AR11" s="15"/>
       <c r="AS11" s="15"/>
@@ -7541,7 +7544,7 @@
       <c r="AY11" s="4"/>
       <c r="AZ11" s="4"/>
       <c r="BA11" s="15"/>
-      <c r="BB11" s="15"/>
+      <c r="BB11" s="36"/>
       <c r="BC11" s="15"/>
       <c r="BD11" s="4"/>
       <c r="BE11" s="4"/>
@@ -7683,9 +7686,9 @@
       <c r="AK12" s="16"/>
       <c r="AL12" s="9"/>
       <c r="AM12" s="9"/>
-      <c r="AN12" s="9"/>
+      <c r="AN12" s="17"/>
       <c r="AO12" s="9"/>
-      <c r="AP12" s="9"/>
+      <c r="AP12" s="17"/>
       <c r="AQ12" s="9"/>
       <c r="AR12" s="17"/>
       <c r="AS12" s="17"/>
@@ -7697,7 +7700,7 @@
       <c r="AY12" s="9"/>
       <c r="AZ12" s="9"/>
       <c r="BA12" s="17"/>
-      <c r="BB12" s="17"/>
+      <c r="BB12" s="9"/>
       <c r="BC12" s="17"/>
       <c r="BD12" s="9"/>
       <c r="BE12" s="9"/>
@@ -7839,9 +7842,9 @@
       <c r="AK13" s="16"/>
       <c r="AL13" s="9"/>
       <c r="AM13" s="9"/>
-      <c r="AN13" s="9"/>
+      <c r="AN13" s="17"/>
       <c r="AO13" s="9"/>
-      <c r="AP13" s="9"/>
+      <c r="AP13" s="17"/>
       <c r="AQ13" s="9"/>
       <c r="AR13" s="17"/>
       <c r="AS13" s="17"/>
@@ -7853,7 +7856,7 @@
       <c r="AY13" s="9"/>
       <c r="AZ13" s="9"/>
       <c r="BA13" s="17"/>
-      <c r="BB13" s="17"/>
+      <c r="BB13" s="9"/>
       <c r="BC13" s="17"/>
       <c r="BD13" s="9"/>
       <c r="BE13" s="9"/>
@@ -7995,9 +7998,9 @@
       <c r="AK14" s="16"/>
       <c r="AL14" s="10"/>
       <c r="AM14" s="10"/>
-      <c r="AN14" s="10"/>
+      <c r="AN14" s="18"/>
       <c r="AO14" s="10"/>
-      <c r="AP14" s="10"/>
+      <c r="AP14" s="18"/>
       <c r="AQ14" s="10"/>
       <c r="AR14" s="18"/>
       <c r="AS14" s="18"/>
@@ -8009,7 +8012,7 @@
       <c r="AY14" s="10"/>
       <c r="AZ14" s="10"/>
       <c r="BA14" s="18"/>
-      <c r="BB14" s="18"/>
+      <c r="BB14" s="10"/>
       <c r="BC14" s="18"/>
       <c r="BD14" s="10"/>
       <c r="BE14" s="10"/>
@@ -8151,9 +8154,9 @@
       <c r="AK15" s="16"/>
       <c r="AL15" s="10"/>
       <c r="AM15" s="10"/>
-      <c r="AN15" s="10"/>
+      <c r="AN15" s="18"/>
       <c r="AO15" s="10"/>
-      <c r="AP15" s="10"/>
+      <c r="AP15" s="18"/>
       <c r="AQ15" s="10"/>
       <c r="AR15" s="18"/>
       <c r="AS15" s="18"/>
@@ -8165,7 +8168,7 @@
       <c r="AY15" s="10"/>
       <c r="AZ15" s="10"/>
       <c r="BA15" s="18"/>
-      <c r="BB15" s="18"/>
+      <c r="BB15" s="10"/>
       <c r="BC15" s="18"/>
       <c r="BD15" s="10"/>
       <c r="BE15" s="10"/>
@@ -8307,9 +8310,9 @@
       <c r="AK16" s="16"/>
       <c r="AL16" s="10"/>
       <c r="AM16" s="10"/>
-      <c r="AN16" s="10"/>
+      <c r="AN16" s="18"/>
       <c r="AO16" s="10"/>
-      <c r="AP16" s="10"/>
+      <c r="AP16" s="18"/>
       <c r="AQ16" s="10"/>
       <c r="AR16" s="18"/>
       <c r="AS16" s="18"/>
@@ -8321,7 +8324,7 @@
       <c r="AY16" s="10"/>
       <c r="AZ16" s="10"/>
       <c r="BA16" s="18"/>
-      <c r="BB16" s="18"/>
+      <c r="BB16" s="10"/>
       <c r="BC16" s="18"/>
       <c r="BD16" s="10"/>
       <c r="BE16" s="10"/>
@@ -8463,9 +8466,9 @@
       <c r="AK17" s="16"/>
       <c r="AL17" s="10"/>
       <c r="AM17" s="10"/>
-      <c r="AN17" s="10"/>
+      <c r="AN17" s="18"/>
       <c r="AO17" s="10"/>
-      <c r="AP17" s="10"/>
+      <c r="AP17" s="18"/>
       <c r="AQ17" s="10"/>
       <c r="AR17" s="18"/>
       <c r="AS17" s="18"/>
@@ -8477,7 +8480,7 @@
       <c r="AY17" s="10"/>
       <c r="AZ17" s="10"/>
       <c r="BA17" s="18"/>
-      <c r="BB17" s="18"/>
+      <c r="BB17" s="10"/>
       <c r="BC17" s="18"/>
       <c r="BD17" s="10"/>
       <c r="BE17" s="10"/>
@@ -8623,9 +8626,9 @@
       <c r="AK18" s="16"/>
       <c r="AL18" s="10"/>
       <c r="AM18" s="10"/>
-      <c r="AN18" s="10"/>
+      <c r="AN18" s="18"/>
       <c r="AO18" s="10"/>
-      <c r="AP18" s="10"/>
+      <c r="AP18" s="18"/>
       <c r="AQ18" s="10"/>
       <c r="AR18" s="18"/>
       <c r="AS18" s="18"/>
@@ -8637,7 +8640,7 @@
       <c r="AY18" s="10"/>
       <c r="AZ18" s="10"/>
       <c r="BA18" s="18"/>
-      <c r="BB18" s="18"/>
+      <c r="BB18" s="10"/>
       <c r="BC18" s="18"/>
       <c r="BD18" s="10"/>
       <c r="BE18" s="10"/>
@@ -8787,9 +8790,9 @@
       <c r="AK19" s="16"/>
       <c r="AL19" s="10"/>
       <c r="AM19" s="10"/>
-      <c r="AN19" s="10"/>
+      <c r="AN19" s="18"/>
       <c r="AO19" s="10"/>
-      <c r="AP19" s="10"/>
+      <c r="AP19" s="18"/>
       <c r="AQ19" s="10"/>
       <c r="AR19" s="18"/>
       <c r="AS19" s="18"/>
@@ -8801,7 +8804,7 @@
       <c r="AY19" s="10"/>
       <c r="AZ19" s="10"/>
       <c r="BA19" s="18"/>
-      <c r="BB19" s="18"/>
+      <c r="BB19" s="10"/>
       <c r="BC19" s="18"/>
       <c r="BD19" s="10"/>
       <c r="BE19" s="10"/>
@@ -8943,9 +8946,9 @@
       <c r="AK20" s="16"/>
       <c r="AL20" s="13"/>
       <c r="AM20" s="13"/>
-      <c r="AN20" s="13"/>
+      <c r="AN20" s="22"/>
       <c r="AO20" s="13"/>
-      <c r="AP20" s="13"/>
+      <c r="AP20" s="22"/>
       <c r="AQ20" s="13"/>
       <c r="AR20" s="22"/>
       <c r="AS20" s="22"/>
@@ -8957,7 +8960,7 @@
       <c r="AY20" s="13"/>
       <c r="AZ20" s="13"/>
       <c r="BA20" s="22"/>
-      <c r="BB20" s="22"/>
+      <c r="BB20" s="13"/>
       <c r="BC20" s="22"/>
       <c r="BD20" s="13"/>
       <c r="BE20" s="13"/>
@@ -10145,16 +10148,16 @@
       </c>
     </row>
     <row r="9" spans="1:185" s="43" customFormat="1">
-      <c r="A9" s="70"/>
-      <c r="B9" s="56"/>
-      <c r="C9" s="56"/>
-      <c r="D9" s="56"/>
-      <c r="E9" s="56"/>
-      <c r="F9" s="56"/>
-      <c r="G9" s="56"/>
-      <c r="H9" s="56"/>
-      <c r="I9" s="56"/>
-      <c r="J9" s="56"/>
+      <c r="A9" s="67"/>
+      <c r="B9" s="55"/>
+      <c r="C9" s="55"/>
+      <c r="D9" s="55"/>
+      <c r="E9" s="55"/>
+      <c r="F9" s="55"/>
+      <c r="G9" s="55"/>
+      <c r="H9" s="55"/>
+      <c r="I9" s="55"/>
+      <c r="J9" s="55"/>
       <c r="K9" s="45" t="s">
         <v>10</v>
       </c>
@@ -10167,7 +10170,7 @@
       </c>
       <c r="O9" s="46"/>
       <c r="P9" s="47"/>
-      <c r="Q9" s="67" t="s">
+      <c r="Q9" s="66" t="s">
         <v>144</v>
       </c>
       <c r="R9" s="46"/>
@@ -10205,30 +10208,30 @@
       <c r="AL9" s="48"/>
       <c r="AM9" s="48"/>
       <c r="AN9" s="53"/>
-      <c r="AO9" s="58" t="s">
+      <c r="AO9" s="57" t="s">
         <v>146</v>
       </c>
-      <c r="AP9" s="56"/>
-      <c r="AQ9" s="56"/>
-      <c r="AR9" s="56"/>
-      <c r="AS9" s="56"/>
-      <c r="AT9" s="56"/>
-      <c r="AU9" s="58" t="s">
+      <c r="AP9" s="55"/>
+      <c r="AQ9" s="55"/>
+      <c r="AR9" s="55"/>
+      <c r="AS9" s="55"/>
+      <c r="AT9" s="55"/>
+      <c r="AU9" s="57" t="s">
         <v>147</v>
       </c>
-      <c r="AV9" s="56"/>
-      <c r="AW9" s="56"/>
-      <c r="AX9" s="56"/>
-      <c r="AY9" s="56"/>
-      <c r="AZ9" s="56"/>
-      <c r="BA9" s="58" t="s">
+      <c r="AV9" s="55"/>
+      <c r="AW9" s="55"/>
+      <c r="AX9" s="55"/>
+      <c r="AY9" s="55"/>
+      <c r="AZ9" s="55"/>
+      <c r="BA9" s="57" t="s">
         <v>148</v>
       </c>
-      <c r="BB9" s="56"/>
-      <c r="BC9" s="56"/>
-      <c r="BD9" s="56"/>
-      <c r="BE9" s="56"/>
-      <c r="BF9" s="56"/>
+      <c r="BB9" s="55"/>
+      <c r="BC9" s="55"/>
+      <c r="BD9" s="55"/>
+      <c r="BE9" s="55"/>
+      <c r="BF9" s="55"/>
       <c r="BG9" s="45" t="s">
         <v>169</v>
       </c>
@@ -10263,7 +10266,7 @@
       <c r="BZ9" s="46"/>
       <c r="CA9" s="46"/>
       <c r="CB9" s="47"/>
-      <c r="CC9" s="55"/>
+      <c r="CC9" s="54"/>
       <c r="CD9" s="49" t="s">
         <v>183</v>
       </c>
@@ -10304,14 +10307,14 @@
       <c r="CW9" s="46"/>
       <c r="CX9" s="46"/>
       <c r="CY9" s="47"/>
-      <c r="CZ9" s="55"/>
-      <c r="DA9" s="56"/>
-      <c r="DB9" s="56"/>
-      <c r="DC9" s="56"/>
-      <c r="DD9" s="56"/>
-      <c r="DE9" s="56"/>
-      <c r="DF9" s="56"/>
-      <c r="DG9" s="55"/>
+      <c r="CZ9" s="54"/>
+      <c r="DA9" s="55"/>
+      <c r="DB9" s="55"/>
+      <c r="DC9" s="55"/>
+      <c r="DD9" s="55"/>
+      <c r="DE9" s="55"/>
+      <c r="DF9" s="55"/>
+      <c r="DG9" s="54"/>
       <c r="DH9" s="45" t="s">
         <v>181</v>
       </c>
@@ -10369,7 +10372,7 @@
       <c r="ET9" s="46"/>
       <c r="EU9" s="46"/>
       <c r="EV9" s="47"/>
-      <c r="EW9" s="61" t="s">
+      <c r="EW9" s="60" t="s">
         <v>86</v>
       </c>
       <c r="EX9" s="51" t="s">
@@ -10382,8 +10385,8 @@
       <c r="FA9" s="46"/>
       <c r="FB9" s="46"/>
       <c r="FC9" s="47"/>
-      <c r="FD9" s="55"/>
-      <c r="FE9" s="57"/>
+      <c r="FD9" s="54"/>
+      <c r="FE9" s="56"/>
       <c r="FF9" s="49" t="s">
         <v>151</v>
       </c>
@@ -10396,14 +10399,14 @@
       <c r="FM9" s="46"/>
       <c r="FN9" s="46"/>
       <c r="FO9" s="47"/>
-      <c r="FP9" s="62"/>
-      <c r="FQ9" s="57"/>
-      <c r="FR9" s="62"/>
-      <c r="FS9" s="57"/>
-      <c r="FT9" s="55"/>
-      <c r="FU9" s="57"/>
-      <c r="FV9" s="55"/>
-      <c r="FW9" s="56"/>
+      <c r="FP9" s="61"/>
+      <c r="FQ9" s="56"/>
+      <c r="FR9" s="61"/>
+      <c r="FS9" s="56"/>
+      <c r="FT9" s="54"/>
+      <c r="FU9" s="56"/>
+      <c r="FV9" s="54"/>
+      <c r="FW9" s="55"/>
       <c r="FX9" s="45" t="s">
         <v>114</v>
       </c>
@@ -10412,563 +10415,563 @@
         <v>115</v>
       </c>
       <c r="GA9" s="47"/>
-      <c r="GB9" s="63"/>
-      <c r="GC9" s="71"/>
+      <c r="GB9" s="62"/>
+      <c r="GC9" s="68"/>
     </row>
     <row r="10" spans="1:185" s="43" customFormat="1">
-      <c r="A10" s="65" t="s">
+      <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>1</v>
       </c>
-      <c r="C10" s="66" t="s">
+      <c r="C10" s="65" t="s">
         <v>2</v>
       </c>
-      <c r="D10" s="66" t="s">
+      <c r="D10" s="65" t="s">
         <v>3</v>
       </c>
-      <c r="E10" s="66" t="s">
+      <c r="E10" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="F10" s="66" t="s">
+      <c r="F10" s="65" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="66" t="s">
+      <c r="G10" s="65" t="s">
         <v>165</v>
       </c>
-      <c r="H10" s="66" t="s">
+      <c r="H10" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="I10" s="66" t="s">
+      <c r="I10" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="66" t="s">
+      <c r="J10" s="65" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="67" t="s">
+      <c r="K10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="L10" s="67" t="s">
+      <c r="L10" s="66" t="s">
         <v>13</v>
       </c>
-      <c r="M10" s="67" t="s">
+      <c r="M10" s="66" t="s">
         <v>14</v>
       </c>
-      <c r="N10" s="67" t="s">
+      <c r="N10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="O10" s="67" t="s">
+      <c r="O10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="P10" s="67" t="s">
+      <c r="P10" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="Q10" s="67" t="s">
+      <c r="Q10" s="66" t="s">
         <v>153</v>
       </c>
-      <c r="R10" s="67" t="s">
+      <c r="R10" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="S10" s="67" t="s">
+      <c r="S10" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="T10" s="67" t="s">
+      <c r="T10" s="66" t="s">
         <v>145</v>
       </c>
-      <c r="U10" s="67" t="s">
+      <c r="U10" s="66" t="s">
         <v>20</v>
       </c>
-      <c r="V10" s="67" t="s">
+      <c r="V10" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="W10" s="67" t="s">
+      <c r="W10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="X10" s="67" t="s">
+      <c r="X10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="Y10" s="67" t="s">
+      <c r="Y10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="Z10" s="67" t="s">
+      <c r="Z10" s="66" t="s">
         <v>23</v>
       </c>
-      <c r="AA10" s="67" t="s">
+      <c r="AA10" s="66" t="s">
         <v>24</v>
       </c>
-      <c r="AB10" s="67" t="s">
+      <c r="AB10" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="AC10" s="67" t="s">
+      <c r="AC10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AD10" s="67" t="s">
+      <c r="AD10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AE10" s="67" t="s">
+      <c r="AE10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AF10" s="67" t="s">
+      <c r="AF10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AG10" s="67" t="s">
+      <c r="AG10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AH10" s="67" t="s">
+      <c r="AH10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AI10" s="67" t="s">
+      <c r="AI10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AJ10" s="67" t="s">
+      <c r="AJ10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AK10" s="67" t="s">
+      <c r="AK10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AL10" s="67" t="s">
+      <c r="AL10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AM10" s="67" t="s">
+      <c r="AM10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AN10" s="67" t="s">
+      <c r="AN10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AO10" s="67" t="s">
+      <c r="AO10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AP10" s="67" t="s">
+      <c r="AP10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AQ10" s="67" t="s">
+      <c r="AQ10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AR10" s="67" t="s">
+      <c r="AR10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AS10" s="67" t="s">
+      <c r="AS10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="AT10" s="67" t="s">
+      <c r="AT10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="AU10" s="67" t="s">
+      <c r="AU10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="AV10" s="67" t="s">
+      <c r="AV10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="AW10" s="67" t="s">
+      <c r="AW10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="AX10" s="67" t="s">
+      <c r="AX10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AY10" s="67" t="s">
+      <c r="AY10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="AZ10" s="67" t="s">
+      <c r="AZ10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BA10" s="67" t="s">
+      <c r="BA10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="BB10" s="67" t="s">
+      <c r="BB10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="BC10" s="67" t="s">
+      <c r="BC10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="BD10" s="67" t="s">
+      <c r="BD10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="BE10" s="67" t="s">
+      <c r="BE10" s="66" t="s">
         <v>133</v>
       </c>
-      <c r="BF10" s="67" t="s">
+      <c r="BF10" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="BG10" s="67" t="s">
+      <c r="BG10" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="BH10" s="67" t="s">
+      <c r="BH10" s="66" t="s">
         <v>175</v>
       </c>
-      <c r="BI10" s="67" t="s">
+      <c r="BI10" s="66" t="s">
         <v>44</v>
       </c>
-      <c r="BJ10" s="67" t="s">
+      <c r="BJ10" s="66" t="s">
         <v>45</v>
       </c>
-      <c r="BK10" s="67" t="s">
+      <c r="BK10" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="BL10" s="67" t="s">
+      <c r="BL10" s="66" t="s">
         <v>46</v>
       </c>
-      <c r="BM10" s="67" t="s">
+      <c r="BM10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="BN10" s="67" t="s">
+      <c r="BN10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="BO10" s="67" t="s">
+      <c r="BO10" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="BP10" s="67" t="s">
+      <c r="BP10" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="BQ10" s="67" t="s">
+      <c r="BQ10" s="66" t="s">
         <v>48</v>
       </c>
-      <c r="BR10" s="67" t="s">
+      <c r="BR10" s="66" t="s">
         <v>49</v>
       </c>
-      <c r="BS10" s="67" t="s">
+      <c r="BS10" s="66" t="s">
         <v>185</v>
       </c>
-      <c r="BT10" s="67" t="s">
+      <c r="BT10" s="66" t="s">
         <v>166</v>
       </c>
-      <c r="BU10" s="67" t="s">
+      <c r="BU10" s="66" t="s">
         <v>51</v>
       </c>
-      <c r="BV10" s="67" t="s">
+      <c r="BV10" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="BW10" s="67" t="s">
+      <c r="BW10" s="66" t="s">
         <v>53</v>
       </c>
-      <c r="BX10" s="67" t="s">
+      <c r="BX10" s="66" t="s">
         <v>54</v>
       </c>
-      <c r="BY10" s="67" t="s">
+      <c r="BY10" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="BZ10" s="67" t="s">
+      <c r="BZ10" s="66" t="s">
         <v>56</v>
       </c>
-      <c r="CA10" s="67" t="s">
+      <c r="CA10" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="CB10" s="67" t="s">
+      <c r="CB10" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="CC10" s="66" t="s">
+      <c r="CC10" s="65" t="s">
         <v>182</v>
       </c>
-      <c r="CD10" s="67" t="s">
+      <c r="CD10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CE10" s="67" t="s">
+      <c r="CE10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CF10" s="67" t="s">
+      <c r="CF10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CG10" s="67" t="s">
+      <c r="CG10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CH10" s="67" t="s">
+      <c r="CH10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="CI10" s="67" t="s">
+      <c r="CI10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="CJ10" s="67" t="s">
+      <c r="CJ10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="CK10" s="67" t="s">
+      <c r="CK10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="CL10" s="67" t="s">
+      <c r="CL10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="CM10" s="67" t="s">
+      <c r="CM10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="CN10" s="67" t="s">
+      <c r="CN10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="CO10" s="67" t="s">
+      <c r="CO10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="CP10" s="67" t="s">
+      <c r="CP10" s="66" t="s">
         <v>62</v>
       </c>
-      <c r="CQ10" s="67" t="s">
+      <c r="CQ10" s="66" t="s">
         <v>186</v>
       </c>
-      <c r="CR10" s="67" t="s">
+      <c r="CR10" s="66" t="s">
         <v>137</v>
       </c>
-      <c r="CS10" s="67" t="s">
+      <c r="CS10" s="66" t="s">
         <v>138</v>
       </c>
-      <c r="CT10" s="67" t="s">
+      <c r="CT10" s="66" t="s">
         <v>139</v>
       </c>
-      <c r="CU10" s="67" t="s">
+      <c r="CU10" s="66" t="s">
         <v>140</v>
       </c>
-      <c r="CV10" s="67" t="s">
+      <c r="CV10" s="66" t="s">
         <v>61</v>
       </c>
-      <c r="CW10" s="67" t="s">
+      <c r="CW10" s="66" t="s">
         <v>187</v>
       </c>
-      <c r="CX10" s="67" t="s">
+      <c r="CX10" s="66" t="s">
         <v>142</v>
       </c>
-      <c r="CY10" s="67" t="s">
+      <c r="CY10" s="66" t="s">
         <v>39</v>
       </c>
-      <c r="CZ10" s="67" t="s">
+      <c r="CZ10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="DA10" s="67" t="s">
+      <c r="DA10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="DB10" s="67" t="s">
+      <c r="DB10" s="66" t="s">
         <v>64</v>
       </c>
-      <c r="DC10" s="67" t="s">
+      <c r="DC10" s="66" t="s">
         <v>65</v>
       </c>
-      <c r="DD10" s="67" t="s">
+      <c r="DD10" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="DE10" s="67" t="s">
+      <c r="DE10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="DF10" s="67" t="s">
+      <c r="DF10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="DG10" s="67" t="s">
+      <c r="DG10" s="66" t="s">
         <v>182</v>
       </c>
-      <c r="DH10" s="67" t="s">
+      <c r="DH10" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="DI10" s="67" t="s">
+      <c r="DI10" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="DJ10" s="67" t="s">
+      <c r="DJ10" s="66" t="s">
         <v>132</v>
       </c>
-      <c r="DK10" s="67" t="s">
+      <c r="DK10" s="66" t="s">
         <v>135</v>
       </c>
-      <c r="DL10" s="67" t="s">
+      <c r="DL10" s="66" t="s">
         <v>69</v>
       </c>
-      <c r="DM10" s="67" t="s">
+      <c r="DM10" s="66" t="s">
         <v>70</v>
       </c>
-      <c r="DN10" s="67" t="s">
+      <c r="DN10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="DO10" s="67" t="s">
+      <c r="DO10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DP10" s="67" t="s">
+      <c r="DP10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DQ10" s="67" t="s">
+      <c r="DQ10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="DR10" s="67" t="s">
+      <c r="DR10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DS10" s="67" t="s">
+      <c r="DS10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DT10" s="67" t="s">
+      <c r="DT10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="DU10" s="67" t="s">
+      <c r="DU10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DV10" s="67" t="s">
+      <c r="DV10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DW10" s="67" t="s">
+      <c r="DW10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="DX10" s="67" t="s">
+      <c r="DX10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="DY10" s="67" t="s">
+      <c r="DY10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="DZ10" s="67" t="s">
+      <c r="DZ10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="EA10" s="67" t="s">
+      <c r="EA10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EB10" s="67" t="s">
+      <c r="EB10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EC10" s="67" t="s">
+      <c r="EC10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="ED10" s="67" t="s">
+      <c r="ED10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EE10" s="67" t="s">
+      <c r="EE10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EF10" s="67" t="s">
+      <c r="EF10" s="66" t="s">
         <v>71</v>
       </c>
-      <c r="EG10" s="67" t="s">
+      <c r="EG10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EH10" s="67" t="s">
+      <c r="EH10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EI10" s="67" t="s">
+      <c r="EI10" s="66" t="s">
         <v>75</v>
       </c>
-      <c r="EJ10" s="67" t="s">
+      <c r="EJ10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EK10" s="67" t="s">
+      <c r="EK10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EL10" s="67" t="s">
+      <c r="EL10" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="EM10" s="67" t="s">
+      <c r="EM10" s="66" t="s">
         <v>72</v>
       </c>
-      <c r="EN10" s="67" t="s">
+      <c r="EN10" s="66" t="s">
         <v>73</v>
       </c>
-      <c r="EO10" s="67" t="s">
+      <c r="EO10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="EP10" s="67" t="s">
+      <c r="EP10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="EQ10" s="67" t="s">
+      <c r="EQ10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="ER10" s="67" t="s">
+      <c r="ER10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="ES10" s="67" t="s">
+      <c r="ES10" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="ET10" s="67" t="s">
+      <c r="ET10" s="66" t="s">
         <v>82</v>
       </c>
-      <c r="EU10" s="67" t="s">
+      <c r="EU10" s="66" t="s">
         <v>83</v>
       </c>
-      <c r="EV10" s="67" t="s">
+      <c r="EV10" s="66" t="s">
         <v>84</v>
       </c>
-      <c r="EW10" s="67" t="s">
+      <c r="EW10" s="66" t="s">
         <v>87</v>
       </c>
-      <c r="EX10" s="67" t="s">
+      <c r="EX10" s="66" t="s">
         <v>88</v>
       </c>
-      <c r="EY10" s="67" t="s">
+      <c r="EY10" s="66" t="s">
         <v>90</v>
       </c>
-      <c r="EZ10" s="67" t="s">
+      <c r="EZ10" s="66" t="s">
         <v>92</v>
       </c>
-      <c r="FA10" s="67" t="s">
+      <c r="FA10" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="FB10" s="67" t="s">
+      <c r="FB10" s="66" t="s">
         <v>94</v>
       </c>
-      <c r="FC10" s="67" t="s">
+      <c r="FC10" s="66" t="s">
         <v>95</v>
       </c>
-      <c r="FD10" s="67" t="s">
+      <c r="FD10" s="66" t="s">
         <v>176</v>
       </c>
-      <c r="FE10" s="67" t="s">
+      <c r="FE10" s="66" t="s">
         <v>97</v>
       </c>
-      <c r="FF10" s="67" t="s">
+      <c r="FF10" s="66" t="s">
         <v>152</v>
       </c>
-      <c r="FG10" s="67" t="s">
+      <c r="FG10" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="FH10" s="67" t="s">
+      <c r="FH10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="FI10" s="67" t="s">
+      <c r="FI10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="FJ10" s="67" t="s">
+      <c r="FJ10" s="66" t="s">
         <v>103</v>
       </c>
       <c r="FK10" s="49" t="s">
         <v>37</v>
       </c>
-      <c r="FL10" s="67" t="s">
+      <c r="FL10" s="66" t="s">
         <v>100</v>
       </c>
-      <c r="FM10" s="67" t="s">
+      <c r="FM10" s="66" t="s">
         <v>101</v>
       </c>
-      <c r="FN10" s="67" t="s">
+      <c r="FN10" s="66" t="s">
         <v>102</v>
       </c>
-      <c r="FO10" s="67" t="s">
+      <c r="FO10" s="66" t="s">
         <v>103</v>
       </c>
-      <c r="FP10" s="66" t="s">
+      <c r="FP10" s="65" t="s">
         <v>105</v>
       </c>
-      <c r="FQ10" s="66" t="s">
+      <c r="FQ10" s="65" t="s">
         <v>106</v>
       </c>
-      <c r="FR10" s="66" t="s">
+      <c r="FR10" s="65" t="s">
         <v>177</v>
       </c>
-      <c r="FS10" s="66" t="s">
+      <c r="FS10" s="65" t="s">
         <v>108</v>
       </c>
-      <c r="FT10" s="67" t="s">
+      <c r="FT10" s="66" t="s">
         <v>110</v>
       </c>
-      <c r="FU10" s="67" t="s">
+      <c r="FU10" s="66" t="s">
         <v>111</v>
       </c>
-      <c r="FV10" s="67" t="s">
+      <c r="FV10" s="66" t="s">
         <v>112</v>
       </c>
-      <c r="FW10" s="67" t="s">
+      <c r="FW10" s="66" t="s">
         <v>113</v>
       </c>
-      <c r="FX10" s="67" t="s">
+      <c r="FX10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="FY10" s="67" t="s">
+      <c r="FY10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="FZ10" s="67" t="s">
+      <c r="FZ10" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="GA10" s="67" t="s">
+      <c r="GA10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="GB10" s="66" t="s">
+      <c r="GB10" s="65" t="s">
         <v>117</v>
       </c>
-      <c r="GC10" s="67" t="s">
+      <c r="GC10" s="66" t="s">
         <v>119</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Change #128879, #128835, #128881
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -1573,6 +1573,15 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="top"/>
+    </xf>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1584,15 +1593,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -3199,7 +3199,7 @@
       <c r="FJ8" s="46"/>
       <c r="FK8" s="46"/>
       <c r="FL8" s="46"/>
-      <c r="FM8" s="75"/>
+      <c r="FM8" s="71"/>
       <c r="FN8" s="45" t="s">
         <v>154</v>
       </c>
@@ -3297,7 +3297,7 @@
       <c r="AN9" s="48"/>
       <c r="AO9" s="48"/>
       <c r="AP9" s="53"/>
-      <c r="AQ9" s="70" t="s">
+      <c r="AQ9" s="73" t="s">
         <v>33</v>
       </c>
       <c r="AR9" s="49" t="s">
@@ -3470,12 +3470,12 @@
       <c r="FE9" s="46"/>
       <c r="FF9" s="46"/>
       <c r="FG9" s="46"/>
-      <c r="FH9" s="74"/>
+      <c r="FH9" s="70"/>
       <c r="FI9" s="48"/>
       <c r="FJ9" s="46"/>
       <c r="FK9" s="46"/>
       <c r="FL9" s="46"/>
-      <c r="FM9" s="75"/>
+      <c r="FM9" s="71"/>
       <c r="FN9" s="61"/>
       <c r="FO9" s="56"/>
       <c r="FP9" s="61"/>
@@ -3494,11 +3494,11 @@
       <c r="FY9" s="47"/>
       <c r="FZ9" s="62"/>
       <c r="GA9" s="54"/>
-      <c r="GB9" s="72" t="s">
+      <c r="GB9" s="75" t="s">
         <v>120</v>
       </c>
       <c r="GC9" s="47"/>
-      <c r="GD9" s="72" t="s">
+      <c r="GD9" s="75" t="s">
         <v>174</v>
       </c>
       <c r="GE9" s="46"/>
@@ -3629,7 +3629,7 @@
       <c r="AP10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AQ10" s="71"/>
+      <c r="AQ10" s="74"/>
       <c r="AR10" s="66" t="s">
         <v>28</v>
       </c>
@@ -4050,11 +4050,11 @@
       <c r="GA10" s="66" t="s">
         <v>119</v>
       </c>
-      <c r="GB10" s="73"/>
+      <c r="GB10" s="76"/>
       <c r="GC10" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="GD10" s="73"/>
+      <c r="GD10" s="76"/>
       <c r="GE10" s="66" t="s">
         <v>122</v>
       </c>
@@ -6864,7 +6864,7 @@
       <c r="EG8" s="46"/>
       <c r="EH8" s="46"/>
       <c r="EI8" s="46"/>
-      <c r="EJ8" s="75"/>
+      <c r="EJ8" s="71"/>
       <c r="EK8" s="45" t="s">
         <v>104</v>
       </c>
@@ -6938,10 +6938,10 @@
         <v>124</v>
       </c>
       <c r="AC9" s="46"/>
-      <c r="AD9" s="70" t="s">
+      <c r="AD9" s="73" t="s">
         <v>130</v>
       </c>
-      <c r="AE9" s="70" t="s">
+      <c r="AE9" s="73" t="s">
         <v>131</v>
       </c>
       <c r="AF9" s="54"/>
@@ -7089,14 +7089,14 @@
         <v>151</v>
       </c>
       <c r="EB9" s="48"/>
-      <c r="EC9" s="74"/>
-      <c r="ED9" s="74"/>
+      <c r="EC9" s="70"/>
+      <c r="ED9" s="70"/>
       <c r="EE9" s="48"/>
       <c r="EF9" s="48"/>
       <c r="EG9" s="48"/>
       <c r="EH9" s="48"/>
       <c r="EI9" s="48"/>
-      <c r="EJ9" s="76"/>
+      <c r="EJ9" s="72"/>
       <c r="EK9" s="61"/>
       <c r="EL9" s="56"/>
       <c r="EM9" s="61"/>
@@ -7202,8 +7202,8 @@
       <c r="AC10" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="AD10" s="71"/>
-      <c r="AE10" s="71"/>
+      <c r="AD10" s="74"/>
+      <c r="AE10" s="74"/>
       <c r="AF10" s="66" t="s">
         <v>132</v>
       </c>
@@ -9208,16 +9208,16 @@
     <col min="16" max="19" width="10.625" style="11"/>
     <col min="20" max="31" width="10.625" style="29"/>
     <col min="32" max="32" width="10.625" style="11"/>
-    <col min="33" max="34" width="10.625" style="29"/>
-    <col min="35" max="36" width="10.625" style="11"/>
-    <col min="37" max="38" width="10.625" style="29"/>
-    <col min="39" max="40" width="10.625" style="11"/>
-    <col min="41" max="42" width="10.625" style="29"/>
-    <col min="43" max="46" width="10.625" style="11"/>
-    <col min="47" max="48" width="10.625" style="29"/>
-    <col min="49" max="52" width="10.625" style="11"/>
-    <col min="53" max="54" width="10.625" style="29"/>
-    <col min="55" max="60" width="10.625" style="11"/>
+    <col min="33" max="35" width="10.625" style="29"/>
+    <col min="36" max="36" width="10.625" style="11"/>
+    <col min="37" max="39" width="10.625" style="29"/>
+    <col min="40" max="40" width="10.625" style="11"/>
+    <col min="41" max="43" width="10.625" style="29"/>
+    <col min="44" max="46" width="10.625" style="11"/>
+    <col min="47" max="49" width="10.625" style="29"/>
+    <col min="50" max="52" width="10.625" style="11"/>
+    <col min="53" max="55" width="10.625" style="29"/>
+    <col min="56" max="60" width="10.625" style="11"/>
     <col min="61" max="61" width="10.625" style="29"/>
     <col min="62" max="62" width="10.625" style="11"/>
     <col min="63" max="63" width="10.625" style="29"/>
@@ -9237,7 +9237,25 @@
     <col min="109" max="109" width="10.625" style="29"/>
     <col min="110" max="111" width="10.625" style="11"/>
     <col min="112" max="115" width="10.625" style="29"/>
-    <col min="116" max="144" width="10.625" style="11"/>
+    <col min="116" max="118" width="10.625" style="11"/>
+    <col min="119" max="119" width="10.625" style="29"/>
+    <col min="120" max="121" width="10.625" style="11"/>
+    <col min="122" max="122" width="10.625" style="29"/>
+    <col min="123" max="124" width="10.625" style="11"/>
+    <col min="125" max="125" width="10.625" style="29"/>
+    <col min="126" max="127" width="10.625" style="11"/>
+    <col min="128" max="128" width="10.625" style="29"/>
+    <col min="129" max="130" width="10.625" style="11"/>
+    <col min="131" max="131" width="10.625" style="29"/>
+    <col min="132" max="133" width="10.625" style="11"/>
+    <col min="134" max="134" width="10.625" style="29"/>
+    <col min="135" max="136" width="10.625" style="11"/>
+    <col min="137" max="137" width="10.625" style="29"/>
+    <col min="138" max="139" width="10.625" style="11"/>
+    <col min="140" max="140" width="10.625" style="29"/>
+    <col min="141" max="142" width="10.625" style="11"/>
+    <col min="143" max="143" width="10.625" style="29"/>
+    <col min="144" max="144" width="10.625" style="11"/>
     <col min="145" max="145" width="10.625" style="29"/>
     <col min="146" max="146" width="10.625" style="11"/>
     <col min="147" max="147" width="10.625" style="29"/>
@@ -9349,6 +9367,7 @@
       <c r="DI1" s="27"/>
       <c r="DJ1" s="27"/>
       <c r="DK1" s="27"/>
+      <c r="DX1" s="27"/>
       <c r="EO1" s="27"/>
       <c r="EQ1" s="27"/>
       <c r="ES1" s="27"/>
@@ -9457,6 +9476,7 @@
       <c r="DI2" s="27"/>
       <c r="DJ2" s="27"/>
       <c r="DK2" s="27"/>
+      <c r="DX2" s="27"/>
       <c r="EO2" s="27"/>
       <c r="EQ2" s="27"/>
       <c r="ES2" s="27"/>
@@ -9565,6 +9585,7 @@
       <c r="DI3" s="27"/>
       <c r="DJ3" s="27"/>
       <c r="DK3" s="27"/>
+      <c r="DX3" s="27"/>
       <c r="EO3" s="27"/>
       <c r="EQ3" s="27"/>
       <c r="ES3" s="27"/>
@@ -9673,6 +9694,7 @@
       <c r="DI4" s="27"/>
       <c r="DJ4" s="27"/>
       <c r="DK4" s="27"/>
+      <c r="DX4" s="27"/>
       <c r="EO4" s="27"/>
       <c r="EQ4" s="27"/>
       <c r="ES4" s="27"/>
@@ -9746,6 +9768,7 @@
       <c r="DI5" s="27"/>
       <c r="DJ5" s="27"/>
       <c r="DK5" s="27"/>
+      <c r="DX5" s="27"/>
       <c r="EO5" s="27"/>
       <c r="EQ5" s="27"/>
       <c r="ES5" s="27"/>
@@ -9799,27 +9822,27 @@
       <c r="AF6"/>
       <c r="AG6" s="28"/>
       <c r="AH6" s="28"/>
-      <c r="AI6"/>
+      <c r="AI6" s="33"/>
       <c r="AJ6"/>
       <c r="AK6" s="28"/>
       <c r="AL6" s="28"/>
-      <c r="AM6"/>
+      <c r="AM6" s="33"/>
       <c r="AN6"/>
       <c r="AO6" s="28"/>
       <c r="AP6" s="28"/>
-      <c r="AQ6"/>
+      <c r="AQ6" s="33"/>
       <c r="AR6"/>
       <c r="AS6"/>
       <c r="AT6"/>
       <c r="AU6" s="28"/>
       <c r="AV6" s="28"/>
-      <c r="AW6"/>
+      <c r="AW6" s="33"/>
       <c r="AX6"/>
       <c r="AY6"/>
       <c r="AZ6"/>
       <c r="BA6" s="28"/>
       <c r="BB6" s="28"/>
-      <c r="BC6"/>
+      <c r="BC6" s="33"/>
       <c r="BD6"/>
       <c r="BE6"/>
       <c r="BF6"/>
@@ -9883,31 +9906,31 @@
       <c r="DL6"/>
       <c r="DM6"/>
       <c r="DN6"/>
-      <c r="DO6"/>
+      <c r="DO6" s="33"/>
       <c r="DP6"/>
       <c r="DQ6"/>
-      <c r="DR6"/>
+      <c r="DR6" s="33"/>
       <c r="DS6"/>
       <c r="DT6"/>
-      <c r="DU6"/>
+      <c r="DU6" s="33"/>
       <c r="DV6"/>
       <c r="DW6"/>
-      <c r="DX6"/>
+      <c r="DX6" s="28"/>
       <c r="DY6"/>
       <c r="DZ6"/>
-      <c r="EA6"/>
+      <c r="EA6" s="33"/>
       <c r="EB6"/>
       <c r="EC6"/>
-      <c r="ED6"/>
+      <c r="ED6" s="33"/>
       <c r="EE6"/>
       <c r="EF6"/>
-      <c r="EG6"/>
+      <c r="EG6" s="33"/>
       <c r="EH6"/>
       <c r="EI6"/>
-      <c r="EJ6"/>
+      <c r="EJ6" s="33"/>
       <c r="EK6"/>
       <c r="EL6"/>
-      <c r="EM6"/>
+      <c r="EM6" s="33"/>
       <c r="EN6"/>
       <c r="EO6" s="28"/>
       <c r="EP6"/>
@@ -10012,6 +10035,7 @@
       <c r="DI7" s="32"/>
       <c r="DJ7" s="32"/>
       <c r="DK7" s="32"/>
+      <c r="DX7" s="32"/>
       <c r="EO7" s="32"/>
       <c r="EQ7" s="32"/>
       <c r="ES7" s="32"/>
@@ -10176,7 +10200,7 @@
       <c r="DU8" s="46"/>
       <c r="DV8" s="46"/>
       <c r="DW8" s="46"/>
-      <c r="DX8" s="46"/>
+      <c r="DX8" s="69"/>
       <c r="DY8" s="46"/>
       <c r="DZ8" s="46"/>
       <c r="EA8" s="46"/>
@@ -10227,7 +10251,7 @@
       <c r="FL8" s="46"/>
       <c r="FM8" s="69"/>
       <c r="FN8" s="69"/>
-      <c r="FO8" s="75"/>
+      <c r="FO8" s="71"/>
       <c r="FP8" s="45" t="s">
         <v>154</v>
       </c>
@@ -10449,7 +10473,7 @@
       <c r="DW9" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="DX9" s="46"/>
+      <c r="DX9" s="69"/>
       <c r="DY9" s="46"/>
       <c r="DZ9" s="46"/>
       <c r="EA9" s="46"/>
@@ -10501,12 +10525,12 @@
       <c r="FG9" s="48"/>
       <c r="FH9" s="48"/>
       <c r="FI9" s="48"/>
-      <c r="FJ9" s="74"/>
+      <c r="FJ9" s="70"/>
       <c r="FK9" s="48"/>
       <c r="FL9" s="48"/>
       <c r="FM9" s="69"/>
       <c r="FN9" s="69"/>
-      <c r="FO9" s="75"/>
+      <c r="FO9" s="71"/>
       <c r="FP9" s="61"/>
       <c r="FQ9" s="56"/>
       <c r="FR9" s="61"/>
@@ -11118,27 +11142,27 @@
       <c r="AF11" s="8"/>
       <c r="AG11" s="25"/>
       <c r="AH11" s="16"/>
-      <c r="AI11" s="8"/>
+      <c r="AI11" s="16"/>
       <c r="AJ11" s="8"/>
       <c r="AK11" s="25"/>
       <c r="AL11" s="16"/>
-      <c r="AM11" s="8"/>
+      <c r="AM11" s="16"/>
       <c r="AN11" s="8"/>
       <c r="AO11" s="16"/>
       <c r="AP11" s="16"/>
-      <c r="AQ11" s="8"/>
+      <c r="AQ11" s="16"/>
       <c r="AR11" s="8"/>
       <c r="AS11" s="8"/>
       <c r="AT11" s="8"/>
       <c r="AU11" s="16"/>
       <c r="AV11" s="16"/>
-      <c r="AW11" s="8"/>
+      <c r="AW11" s="16"/>
       <c r="AX11" s="8"/>
       <c r="AY11" s="8"/>
       <c r="AZ11" s="8"/>
       <c r="BA11" s="16"/>
       <c r="BB11" s="16"/>
-      <c r="BC11" s="8"/>
+      <c r="BC11" s="16"/>
       <c r="BD11" s="8"/>
       <c r="BE11" s="8"/>
       <c r="BF11" s="8"/>
@@ -11201,31 +11225,31 @@
       <c r="DL11" s="4"/>
       <c r="DM11" s="4"/>
       <c r="DN11" s="4"/>
-      <c r="DO11" s="4"/>
+      <c r="DO11" s="15"/>
       <c r="DP11" s="4"/>
       <c r="DQ11" s="4"/>
-      <c r="DR11" s="4"/>
+      <c r="DR11" s="15"/>
       <c r="DS11" s="4"/>
       <c r="DT11" s="4"/>
-      <c r="DU11" s="4"/>
+      <c r="DU11" s="15"/>
       <c r="DV11" s="4"/>
       <c r="DW11" s="4"/>
-      <c r="DX11" s="4"/>
+      <c r="DX11" s="15"/>
       <c r="DY11" s="4"/>
       <c r="DZ11" s="4"/>
-      <c r="EA11" s="4"/>
+      <c r="EA11" s="15"/>
       <c r="EB11" s="4"/>
       <c r="EC11" s="4"/>
-      <c r="ED11" s="4"/>
+      <c r="ED11" s="15"/>
       <c r="EE11" s="4"/>
       <c r="EF11" s="4"/>
-      <c r="EG11" s="4"/>
+      <c r="EG11" s="15"/>
       <c r="EH11" s="4"/>
       <c r="EI11" s="4"/>
-      <c r="EJ11" s="4"/>
+      <c r="EJ11" s="15"/>
       <c r="EK11" s="4"/>
       <c r="EL11" s="4"/>
-      <c r="EM11" s="4"/>
+      <c r="EM11" s="15"/>
       <c r="EN11" s="4"/>
       <c r="EO11" s="15"/>
       <c r="EP11" s="4"/>
@@ -11304,27 +11328,27 @@
       <c r="AF12" s="8"/>
       <c r="AG12" s="25"/>
       <c r="AH12" s="16"/>
-      <c r="AI12" s="8"/>
+      <c r="AI12" s="16"/>
       <c r="AJ12" s="8"/>
       <c r="AK12" s="25"/>
       <c r="AL12" s="16"/>
-      <c r="AM12" s="8"/>
+      <c r="AM12" s="16"/>
       <c r="AN12" s="8"/>
       <c r="AO12" s="16"/>
       <c r="AP12" s="16"/>
-      <c r="AQ12" s="8"/>
+      <c r="AQ12" s="16"/>
       <c r="AR12" s="8"/>
       <c r="AS12" s="8"/>
       <c r="AT12" s="8"/>
       <c r="AU12" s="16"/>
       <c r="AV12" s="16"/>
-      <c r="AW12" s="8"/>
+      <c r="AW12" s="16"/>
       <c r="AX12" s="8"/>
       <c r="AY12" s="8"/>
       <c r="AZ12" s="8"/>
       <c r="BA12" s="16"/>
       <c r="BB12" s="16"/>
-      <c r="BC12" s="8"/>
+      <c r="BC12" s="16"/>
       <c r="BD12" s="8"/>
       <c r="BE12" s="8"/>
       <c r="BF12" s="8"/>
@@ -11387,31 +11411,31 @@
       <c r="DL12" s="9"/>
       <c r="DM12" s="9"/>
       <c r="DN12" s="9"/>
-      <c r="DO12" s="9"/>
+      <c r="DO12" s="17"/>
       <c r="DP12" s="9"/>
       <c r="DQ12" s="9"/>
-      <c r="DR12" s="9"/>
+      <c r="DR12" s="17"/>
       <c r="DS12" s="9"/>
       <c r="DT12" s="9"/>
-      <c r="DU12" s="9"/>
+      <c r="DU12" s="17"/>
       <c r="DV12" s="9"/>
       <c r="DW12" s="9"/>
-      <c r="DX12" s="9"/>
+      <c r="DX12" s="17"/>
       <c r="DY12" s="9"/>
       <c r="DZ12" s="9"/>
-      <c r="EA12" s="9"/>
+      <c r="EA12" s="17"/>
       <c r="EB12" s="9"/>
       <c r="EC12" s="9"/>
-      <c r="ED12" s="9"/>
+      <c r="ED12" s="17"/>
       <c r="EE12" s="9"/>
       <c r="EF12" s="9"/>
-      <c r="EG12" s="9"/>
+      <c r="EG12" s="17"/>
       <c r="EH12" s="9"/>
       <c r="EI12" s="9"/>
-      <c r="EJ12" s="9"/>
+      <c r="EJ12" s="17"/>
       <c r="EK12" s="9"/>
       <c r="EL12" s="9"/>
-      <c r="EM12" s="9"/>
+      <c r="EM12" s="17"/>
       <c r="EN12" s="9"/>
       <c r="EO12" s="17"/>
       <c r="EP12" s="9"/>
@@ -11490,27 +11514,27 @@
       <c r="AF13" s="8"/>
       <c r="AG13" s="25"/>
       <c r="AH13" s="16"/>
-      <c r="AI13" s="8"/>
+      <c r="AI13" s="16"/>
       <c r="AJ13" s="8"/>
       <c r="AK13" s="25"/>
       <c r="AL13" s="16"/>
-      <c r="AM13" s="8"/>
+      <c r="AM13" s="16"/>
       <c r="AN13" s="8"/>
       <c r="AO13" s="16"/>
       <c r="AP13" s="16"/>
-      <c r="AQ13" s="8"/>
+      <c r="AQ13" s="16"/>
       <c r="AR13" s="8"/>
       <c r="AS13" s="8"/>
       <c r="AT13" s="8"/>
       <c r="AU13" s="16"/>
       <c r="AV13" s="16"/>
-      <c r="AW13" s="8"/>
+      <c r="AW13" s="16"/>
       <c r="AX13" s="8"/>
       <c r="AY13" s="8"/>
       <c r="AZ13" s="8"/>
       <c r="BA13" s="16"/>
       <c r="BB13" s="16"/>
-      <c r="BC13" s="8"/>
+      <c r="BC13" s="16"/>
       <c r="BD13" s="8"/>
       <c r="BE13" s="8"/>
       <c r="BF13" s="8"/>
@@ -11574,31 +11598,31 @@
       <c r="DL13" s="10"/>
       <c r="DM13" s="10"/>
       <c r="DN13" s="10"/>
-      <c r="DO13" s="10"/>
+      <c r="DO13" s="18"/>
       <c r="DP13" s="10"/>
       <c r="DQ13" s="10"/>
-      <c r="DR13" s="10"/>
+      <c r="DR13" s="18"/>
       <c r="DS13" s="10"/>
       <c r="DT13" s="10"/>
-      <c r="DU13" s="10"/>
+      <c r="DU13" s="18"/>
       <c r="DV13" s="10"/>
       <c r="DW13" s="10"/>
-      <c r="DX13" s="10"/>
+      <c r="DX13" s="18"/>
       <c r="DY13" s="10"/>
       <c r="DZ13" s="10"/>
-      <c r="EA13" s="10"/>
+      <c r="EA13" s="18"/>
       <c r="EB13" s="10"/>
       <c r="EC13" s="10"/>
-      <c r="ED13" s="10"/>
+      <c r="ED13" s="18"/>
       <c r="EE13" s="10"/>
       <c r="EF13" s="10"/>
-      <c r="EG13" s="10"/>
+      <c r="EG13" s="18"/>
       <c r="EH13" s="10"/>
       <c r="EI13" s="10"/>
-      <c r="EJ13" s="10"/>
+      <c r="EJ13" s="18"/>
       <c r="EK13" s="10"/>
       <c r="EL13" s="10"/>
-      <c r="EM13" s="10"/>
+      <c r="EM13" s="18"/>
       <c r="EN13" s="10"/>
       <c r="EO13" s="18"/>
       <c r="EP13" s="10"/>
@@ -11677,27 +11701,27 @@
       <c r="AF14" s="8"/>
       <c r="AG14" s="25"/>
       <c r="AH14" s="16"/>
-      <c r="AI14" s="8"/>
+      <c r="AI14" s="16"/>
       <c r="AJ14" s="8"/>
       <c r="AK14" s="25"/>
       <c r="AL14" s="16"/>
-      <c r="AM14" s="8"/>
+      <c r="AM14" s="16"/>
       <c r="AN14" s="8"/>
       <c r="AO14" s="16"/>
       <c r="AP14" s="16"/>
-      <c r="AQ14" s="8"/>
+      <c r="AQ14" s="16"/>
       <c r="AR14" s="8"/>
       <c r="AS14" s="8"/>
       <c r="AT14" s="8"/>
       <c r="AU14" s="16"/>
       <c r="AV14" s="16"/>
-      <c r="AW14" s="8"/>
+      <c r="AW14" s="16"/>
       <c r="AX14" s="8"/>
       <c r="AY14" s="8"/>
       <c r="AZ14" s="8"/>
       <c r="BA14" s="16"/>
       <c r="BB14" s="16"/>
-      <c r="BC14" s="8"/>
+      <c r="BC14" s="16"/>
       <c r="BD14" s="8"/>
       <c r="BE14" s="8"/>
       <c r="BF14" s="8"/>
@@ -11761,31 +11785,31 @@
       <c r="DL14" s="10"/>
       <c r="DM14" s="10"/>
       <c r="DN14" s="10"/>
-      <c r="DO14" s="10"/>
+      <c r="DO14" s="18"/>
       <c r="DP14" s="10"/>
       <c r="DQ14" s="10"/>
-      <c r="DR14" s="10"/>
+      <c r="DR14" s="18"/>
       <c r="DS14" s="10"/>
       <c r="DT14" s="10"/>
-      <c r="DU14" s="10"/>
+      <c r="DU14" s="18"/>
       <c r="DV14" s="10"/>
       <c r="DW14" s="10"/>
-      <c r="DX14" s="10"/>
+      <c r="DX14" s="18"/>
       <c r="DY14" s="10"/>
       <c r="DZ14" s="10"/>
-      <c r="EA14" s="10"/>
+      <c r="EA14" s="18"/>
       <c r="EB14" s="10"/>
       <c r="EC14" s="10"/>
-      <c r="ED14" s="10"/>
+      <c r="ED14" s="18"/>
       <c r="EE14" s="10"/>
       <c r="EF14" s="10"/>
-      <c r="EG14" s="10"/>
+      <c r="EG14" s="18"/>
       <c r="EH14" s="10"/>
       <c r="EI14" s="10"/>
-      <c r="EJ14" s="10"/>
+      <c r="EJ14" s="18"/>
       <c r="EK14" s="10"/>
       <c r="EL14" s="10"/>
-      <c r="EM14" s="10"/>
+      <c r="EM14" s="18"/>
       <c r="EN14" s="10"/>
       <c r="EO14" s="18"/>
       <c r="EP14" s="10"/>
@@ -11864,27 +11888,27 @@
       <c r="AF15" s="8"/>
       <c r="AG15" s="25"/>
       <c r="AH15" s="16"/>
-      <c r="AI15" s="8"/>
+      <c r="AI15" s="16"/>
       <c r="AJ15" s="8"/>
       <c r="AK15" s="25"/>
       <c r="AL15" s="16"/>
-      <c r="AM15" s="8"/>
+      <c r="AM15" s="16"/>
       <c r="AN15" s="8"/>
       <c r="AO15" s="16"/>
       <c r="AP15" s="16"/>
-      <c r="AQ15" s="8"/>
+      <c r="AQ15" s="16"/>
       <c r="AR15" s="8"/>
       <c r="AS15" s="8"/>
       <c r="AT15" s="8"/>
       <c r="AU15" s="16"/>
       <c r="AV15" s="16"/>
-      <c r="AW15" s="8"/>
+      <c r="AW15" s="16"/>
       <c r="AX15" s="8"/>
       <c r="AY15" s="8"/>
       <c r="AZ15" s="8"/>
       <c r="BA15" s="16"/>
       <c r="BB15" s="16"/>
-      <c r="BC15" s="8"/>
+      <c r="BC15" s="16"/>
       <c r="BD15" s="8"/>
       <c r="BE15" s="8"/>
       <c r="BF15" s="8"/>
@@ -11948,31 +11972,31 @@
       <c r="DL15" s="10"/>
       <c r="DM15" s="10"/>
       <c r="DN15" s="10"/>
-      <c r="DO15" s="10"/>
+      <c r="DO15" s="18"/>
       <c r="DP15" s="10"/>
       <c r="DQ15" s="10"/>
-      <c r="DR15" s="10"/>
+      <c r="DR15" s="18"/>
       <c r="DS15" s="10"/>
       <c r="DT15" s="10"/>
-      <c r="DU15" s="10"/>
+      <c r="DU15" s="18"/>
       <c r="DV15" s="10"/>
       <c r="DW15" s="10"/>
-      <c r="DX15" s="10"/>
+      <c r="DX15" s="18"/>
       <c r="DY15" s="10"/>
       <c r="DZ15" s="10"/>
-      <c r="EA15" s="10"/>
+      <c r="EA15" s="18"/>
       <c r="EB15" s="10"/>
       <c r="EC15" s="10"/>
-      <c r="ED15" s="10"/>
+      <c r="ED15" s="18"/>
       <c r="EE15" s="10"/>
       <c r="EF15" s="10"/>
-      <c r="EG15" s="10"/>
+      <c r="EG15" s="18"/>
       <c r="EH15" s="10"/>
       <c r="EI15" s="10"/>
-      <c r="EJ15" s="10"/>
+      <c r="EJ15" s="18"/>
       <c r="EK15" s="10"/>
       <c r="EL15" s="10"/>
-      <c r="EM15" s="10"/>
+      <c r="EM15" s="18"/>
       <c r="EN15" s="10"/>
       <c r="EO15" s="18"/>
       <c r="EP15" s="10"/>
@@ -12051,27 +12075,27 @@
       <c r="AF16" s="12"/>
       <c r="AG16" s="30"/>
       <c r="AH16" s="30"/>
-      <c r="AI16" s="12"/>
+      <c r="AI16" s="30"/>
       <c r="AJ16" s="12"/>
       <c r="AK16" s="30"/>
       <c r="AL16" s="30"/>
-      <c r="AM16" s="12"/>
+      <c r="AM16" s="30"/>
       <c r="AN16" s="12"/>
       <c r="AO16" s="16"/>
       <c r="AP16" s="16"/>
-      <c r="AQ16" s="8"/>
+      <c r="AQ16" s="16"/>
       <c r="AR16" s="8"/>
       <c r="AS16" s="8"/>
       <c r="AT16" s="8"/>
       <c r="AU16" s="16"/>
       <c r="AV16" s="16"/>
-      <c r="AW16" s="8"/>
+      <c r="AW16" s="16"/>
       <c r="AX16" s="8"/>
       <c r="AY16" s="8"/>
       <c r="AZ16" s="8"/>
       <c r="BA16" s="16"/>
       <c r="BB16" s="16"/>
-      <c r="BC16" s="8"/>
+      <c r="BC16" s="16"/>
       <c r="BD16" s="8"/>
       <c r="BE16" s="8"/>
       <c r="BF16" s="8"/>
@@ -12135,31 +12159,31 @@
       <c r="DL16" s="10"/>
       <c r="DM16" s="10"/>
       <c r="DN16" s="10"/>
-      <c r="DO16" s="10"/>
+      <c r="DO16" s="18"/>
       <c r="DP16" s="10"/>
       <c r="DQ16" s="10"/>
-      <c r="DR16" s="10"/>
+      <c r="DR16" s="18"/>
       <c r="DS16" s="10"/>
       <c r="DT16" s="10"/>
-      <c r="DU16" s="10"/>
+      <c r="DU16" s="18"/>
       <c r="DV16" s="10"/>
       <c r="DW16" s="10"/>
-      <c r="DX16" s="10"/>
+      <c r="DX16" s="18"/>
       <c r="DY16" s="10"/>
       <c r="DZ16" s="10"/>
-      <c r="EA16" s="10"/>
+      <c r="EA16" s="18"/>
       <c r="EB16" s="10"/>
       <c r="EC16" s="10"/>
-      <c r="ED16" s="10"/>
+      <c r="ED16" s="18"/>
       <c r="EE16" s="10"/>
       <c r="EF16" s="10"/>
-      <c r="EG16" s="10"/>
+      <c r="EG16" s="18"/>
       <c r="EH16" s="10"/>
       <c r="EI16" s="10"/>
-      <c r="EJ16" s="10"/>
+      <c r="EJ16" s="18"/>
       <c r="EK16" s="10"/>
       <c r="EL16" s="10"/>
-      <c r="EM16" s="10"/>
+      <c r="EM16" s="18"/>
       <c r="EN16" s="10"/>
       <c r="EO16" s="18"/>
       <c r="EP16" s="10"/>
@@ -12238,27 +12262,27 @@
       <c r="AF17" s="12"/>
       <c r="AG17" s="30"/>
       <c r="AH17" s="30"/>
-      <c r="AI17" s="12"/>
+      <c r="AI17" s="30"/>
       <c r="AJ17" s="12"/>
       <c r="AK17" s="30"/>
       <c r="AL17" s="30"/>
-      <c r="AM17" s="12"/>
+      <c r="AM17" s="30"/>
       <c r="AN17" s="12"/>
       <c r="AO17" s="16"/>
       <c r="AP17" s="16"/>
-      <c r="AQ17" s="8"/>
+      <c r="AQ17" s="16"/>
       <c r="AR17" s="8"/>
       <c r="AS17" s="8"/>
       <c r="AT17" s="8"/>
       <c r="AU17" s="16"/>
       <c r="AV17" s="16"/>
-      <c r="AW17" s="8"/>
+      <c r="AW17" s="16"/>
       <c r="AX17" s="8"/>
       <c r="AY17" s="8"/>
       <c r="AZ17" s="8"/>
       <c r="BA17" s="16"/>
       <c r="BB17" s="16"/>
-      <c r="BC17" s="8"/>
+      <c r="BC17" s="16"/>
       <c r="BD17" s="8"/>
       <c r="BE17" s="8"/>
       <c r="BF17" s="8"/>
@@ -12330,31 +12354,31 @@
       <c r="DL17" s="10"/>
       <c r="DM17" s="10"/>
       <c r="DN17" s="10"/>
-      <c r="DO17" s="10"/>
+      <c r="DO17" s="18"/>
       <c r="DP17" s="10"/>
       <c r="DQ17" s="10"/>
-      <c r="DR17" s="10"/>
+      <c r="DR17" s="18"/>
       <c r="DS17" s="10"/>
       <c r="DT17" s="10"/>
-      <c r="DU17" s="10"/>
+      <c r="DU17" s="18"/>
       <c r="DV17" s="10"/>
       <c r="DW17" s="10"/>
-      <c r="DX17" s="10"/>
+      <c r="DX17" s="18"/>
       <c r="DY17" s="10"/>
       <c r="DZ17" s="10"/>
-      <c r="EA17" s="10"/>
+      <c r="EA17" s="18"/>
       <c r="EB17" s="10"/>
       <c r="EC17" s="10"/>
-      <c r="ED17" s="10"/>
+      <c r="ED17" s="18"/>
       <c r="EE17" s="10"/>
       <c r="EF17" s="10"/>
-      <c r="EG17" s="10"/>
+      <c r="EG17" s="18"/>
       <c r="EH17" s="10"/>
       <c r="EI17" s="10"/>
-      <c r="EJ17" s="10"/>
+      <c r="EJ17" s="18"/>
       <c r="EK17" s="10"/>
       <c r="EL17" s="10"/>
-      <c r="EM17" s="10"/>
+      <c r="EM17" s="18"/>
       <c r="EN17" s="10"/>
       <c r="EO17" s="18"/>
       <c r="EP17" s="10"/>
@@ -12433,27 +12457,27 @@
       <c r="AF18" s="12"/>
       <c r="AG18" s="30"/>
       <c r="AH18" s="30"/>
-      <c r="AI18" s="12"/>
+      <c r="AI18" s="30"/>
       <c r="AJ18" s="12"/>
       <c r="AK18" s="30"/>
       <c r="AL18" s="30"/>
-      <c r="AM18" s="12"/>
+      <c r="AM18" s="30"/>
       <c r="AN18" s="12"/>
       <c r="AO18" s="16"/>
       <c r="AP18" s="16"/>
-      <c r="AQ18" s="8"/>
+      <c r="AQ18" s="16"/>
       <c r="AR18" s="8"/>
       <c r="AS18" s="8"/>
       <c r="AT18" s="8"/>
       <c r="AU18" s="16"/>
       <c r="AV18" s="16"/>
-      <c r="AW18" s="8"/>
+      <c r="AW18" s="16"/>
       <c r="AX18" s="8"/>
       <c r="AY18" s="8"/>
       <c r="AZ18" s="8"/>
       <c r="BA18" s="16"/>
       <c r="BB18" s="16"/>
-      <c r="BC18" s="8"/>
+      <c r="BC18" s="16"/>
       <c r="BD18" s="8"/>
       <c r="BE18" s="8"/>
       <c r="BF18" s="8"/>
@@ -12533,31 +12557,31 @@
       <c r="DL18" s="10"/>
       <c r="DM18" s="10"/>
       <c r="DN18" s="10"/>
-      <c r="DO18" s="10"/>
+      <c r="DO18" s="18"/>
       <c r="DP18" s="10"/>
       <c r="DQ18" s="10"/>
-      <c r="DR18" s="10"/>
+      <c r="DR18" s="18"/>
       <c r="DS18" s="10"/>
       <c r="DT18" s="10"/>
-      <c r="DU18" s="10"/>
+      <c r="DU18" s="18"/>
       <c r="DV18" s="10"/>
       <c r="DW18" s="10"/>
-      <c r="DX18" s="10"/>
+      <c r="DX18" s="18"/>
       <c r="DY18" s="10"/>
       <c r="DZ18" s="10"/>
-      <c r="EA18" s="10"/>
+      <c r="EA18" s="18"/>
       <c r="EB18" s="10"/>
       <c r="EC18" s="10"/>
-      <c r="ED18" s="10"/>
+      <c r="ED18" s="18"/>
       <c r="EE18" s="10"/>
       <c r="EF18" s="10"/>
-      <c r="EG18" s="10"/>
+      <c r="EG18" s="18"/>
       <c r="EH18" s="10"/>
       <c r="EI18" s="10"/>
-      <c r="EJ18" s="10"/>
+      <c r="EJ18" s="18"/>
       <c r="EK18" s="10"/>
       <c r="EL18" s="10"/>
-      <c r="EM18" s="10"/>
+      <c r="EM18" s="18"/>
       <c r="EN18" s="10"/>
       <c r="EO18" s="18"/>
       <c r="EP18" s="10"/>
@@ -12636,27 +12660,27 @@
       <c r="AF19" s="12"/>
       <c r="AG19" s="30"/>
       <c r="AH19" s="30"/>
-      <c r="AI19" s="12"/>
+      <c r="AI19" s="30"/>
       <c r="AJ19" s="12"/>
       <c r="AK19" s="30"/>
       <c r="AL19" s="30"/>
-      <c r="AM19" s="12"/>
+      <c r="AM19" s="30"/>
       <c r="AN19" s="12"/>
       <c r="AO19" s="16"/>
       <c r="AP19" s="16"/>
-      <c r="AQ19" s="8"/>
+      <c r="AQ19" s="16"/>
       <c r="AR19" s="8"/>
       <c r="AS19" s="8"/>
       <c r="AT19" s="8"/>
       <c r="AU19" s="16"/>
       <c r="AV19" s="16"/>
-      <c r="AW19" s="8"/>
+      <c r="AW19" s="16"/>
       <c r="AX19" s="8"/>
       <c r="AY19" s="8"/>
       <c r="AZ19" s="8"/>
       <c r="BA19" s="16"/>
       <c r="BB19" s="16"/>
-      <c r="BC19" s="8"/>
+      <c r="BC19" s="16"/>
       <c r="BD19" s="8"/>
       <c r="BE19" s="8"/>
       <c r="BF19" s="8"/>
@@ -12720,31 +12744,31 @@
       <c r="DL19" s="10"/>
       <c r="DM19" s="10"/>
       <c r="DN19" s="10"/>
-      <c r="DO19" s="10"/>
+      <c r="DO19" s="18"/>
       <c r="DP19" s="10"/>
       <c r="DQ19" s="10"/>
-      <c r="DR19" s="10"/>
+      <c r="DR19" s="18"/>
       <c r="DS19" s="10"/>
       <c r="DT19" s="10"/>
-      <c r="DU19" s="10"/>
+      <c r="DU19" s="18"/>
       <c r="DV19" s="10"/>
       <c r="DW19" s="10"/>
-      <c r="DX19" s="10"/>
+      <c r="DX19" s="18"/>
       <c r="DY19" s="10"/>
       <c r="DZ19" s="10"/>
-      <c r="EA19" s="10"/>
+      <c r="EA19" s="18"/>
       <c r="EB19" s="10"/>
       <c r="EC19" s="10"/>
-      <c r="ED19" s="10"/>
+      <c r="ED19" s="18"/>
       <c r="EE19" s="10"/>
       <c r="EF19" s="10"/>
-      <c r="EG19" s="10"/>
+      <c r="EG19" s="18"/>
       <c r="EH19" s="10"/>
       <c r="EI19" s="10"/>
-      <c r="EJ19" s="10"/>
+      <c r="EJ19" s="18"/>
       <c r="EK19" s="10"/>
       <c r="EL19" s="10"/>
-      <c r="EM19" s="10"/>
+      <c r="EM19" s="18"/>
       <c r="EN19" s="10"/>
       <c r="EO19" s="18"/>
       <c r="EP19" s="10"/>
@@ -12823,27 +12847,27 @@
       <c r="AF20" s="14"/>
       <c r="AG20" s="31"/>
       <c r="AH20" s="31"/>
-      <c r="AI20" s="14"/>
+      <c r="AI20" s="31"/>
       <c r="AJ20" s="14"/>
       <c r="AK20" s="31"/>
       <c r="AL20" s="31"/>
-      <c r="AM20" s="14"/>
+      <c r="AM20" s="31"/>
       <c r="AN20" s="14"/>
       <c r="AO20" s="16"/>
       <c r="AP20" s="16"/>
-      <c r="AQ20" s="8"/>
+      <c r="AQ20" s="16"/>
       <c r="AR20" s="8"/>
       <c r="AS20" s="8"/>
       <c r="AT20" s="8"/>
       <c r="AU20" s="16"/>
       <c r="AV20" s="16"/>
-      <c r="AW20" s="8"/>
+      <c r="AW20" s="16"/>
       <c r="AX20" s="8"/>
       <c r="AY20" s="8"/>
       <c r="AZ20" s="8"/>
       <c r="BA20" s="16"/>
       <c r="BB20" s="16"/>
-      <c r="BC20" s="8"/>
+      <c r="BC20" s="16"/>
       <c r="BD20" s="8"/>
       <c r="BE20" s="8"/>
       <c r="BF20" s="8"/>
@@ -12907,31 +12931,31 @@
       <c r="DL20" s="13"/>
       <c r="DM20" s="13"/>
       <c r="DN20" s="13"/>
-      <c r="DO20" s="13"/>
+      <c r="DO20" s="22"/>
       <c r="DP20" s="13"/>
       <c r="DQ20" s="13"/>
-      <c r="DR20" s="13"/>
+      <c r="DR20" s="22"/>
       <c r="DS20" s="13"/>
       <c r="DT20" s="13"/>
-      <c r="DU20" s="13"/>
+      <c r="DU20" s="22"/>
       <c r="DV20" s="13"/>
       <c r="DW20" s="13"/>
-      <c r="DX20" s="13"/>
+      <c r="DX20" s="22"/>
       <c r="DY20" s="13"/>
       <c r="DZ20" s="13"/>
-      <c r="EA20" s="13"/>
+      <c r="EA20" s="22"/>
       <c r="EB20" s="13"/>
       <c r="EC20" s="13"/>
-      <c r="ED20" s="13"/>
+      <c r="ED20" s="22"/>
       <c r="EE20" s="13"/>
       <c r="EF20" s="13"/>
-      <c r="EG20" s="13"/>
+      <c r="EG20" s="22"/>
       <c r="EH20" s="13"/>
       <c r="EI20" s="13"/>
-      <c r="EJ20" s="13"/>
+      <c r="EJ20" s="22"/>
       <c r="EK20" s="13"/>
       <c r="EL20" s="13"/>
-      <c r="EM20" s="13"/>
+      <c r="EM20" s="22"/>
       <c r="EN20" s="13"/>
       <c r="EO20" s="22"/>
       <c r="EP20" s="13"/>

</xml_diff>

<commit_message>
KMK003 #129253 & #129256
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
@@ -1133,21 +1133,21 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1953,91 +1953,91 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GF20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="11" width="10.625" style="11"/>
-    <col min="12" max="13" width="10.625" style="29"/>
-    <col min="14" max="14" width="10.625" style="11"/>
-    <col min="15" max="18" width="10.625" style="29"/>
-    <col min="19" max="20" width="10.625" style="11"/>
-    <col min="21" max="33" width="10.625" style="29"/>
-    <col min="34" max="34" width="10.625" style="11"/>
-    <col min="35" max="37" width="10.625" style="29"/>
-    <col min="38" max="38" width="10.625" style="11"/>
-    <col min="39" max="41" width="10.625" style="29"/>
-    <col min="42" max="43" width="10.625" style="11"/>
-    <col min="44" max="46" width="10.625" style="29"/>
-    <col min="47" max="51" width="10.625" style="11"/>
-    <col min="52" max="55" width="10.625" style="29"/>
-    <col min="56" max="60" width="10.625" style="11"/>
-    <col min="61" max="64" width="10.625" style="29"/>
-    <col min="65" max="69" width="10.625" style="11"/>
-    <col min="70" max="70" width="10.625" style="29"/>
-    <col min="71" max="72" width="10.625" style="11"/>
-    <col min="73" max="73" width="10.625" style="29"/>
-    <col min="74" max="74" width="10.625" style="11"/>
-    <col min="75" max="75" width="10.625" style="29"/>
-    <col min="76" max="76" width="10.625" style="11"/>
-    <col min="77" max="84" width="10.625" style="29"/>
-    <col min="85" max="88" width="10.625" style="11"/>
-    <col min="89" max="89" width="10.625" style="29"/>
-    <col min="90" max="90" width="10.625" style="11"/>
-    <col min="91" max="91" width="10.625" style="29"/>
-    <col min="92" max="92" width="10.625" style="11"/>
-    <col min="93" max="94" width="10.625" style="29"/>
-    <col min="95" max="95" width="10.625" style="11"/>
-    <col min="96" max="97" width="10.625" style="29"/>
-    <col min="98" max="98" width="10.625" style="11"/>
-    <col min="99" max="100" width="10.625" style="29"/>
-    <col min="101" max="103" width="10.625" style="11"/>
-    <col min="104" max="105" width="10.625" style="29"/>
-    <col min="106" max="108" width="10.625" style="11"/>
-    <col min="109" max="109" width="10.625" style="29"/>
-    <col min="110" max="110" width="10.625" style="11"/>
-    <col min="111" max="112" width="10.625" style="29"/>
-    <col min="113" max="116" width="10.625" style="11"/>
-    <col min="117" max="117" width="10.625" style="29"/>
-    <col min="118" max="119" width="10.625" style="11"/>
-    <col min="120" max="120" width="10.625" style="29"/>
-    <col min="121" max="122" width="10.625" style="11"/>
-    <col min="123" max="123" width="10.625" style="29"/>
-    <col min="124" max="125" width="10.625" style="11"/>
-    <col min="126" max="126" width="10.625" style="29"/>
-    <col min="127" max="128" width="10.625" style="11"/>
-    <col min="129" max="129" width="10.625" style="29"/>
-    <col min="130" max="131" width="10.625" style="11"/>
-    <col min="132" max="132" width="10.625" style="29"/>
-    <col min="133" max="134" width="10.625" style="11"/>
-    <col min="135" max="135" width="10.625" style="29"/>
-    <col min="136" max="137" width="10.625" style="11"/>
-    <col min="138" max="138" width="10.625" style="29"/>
-    <col min="139" max="140" width="10.625" style="11"/>
-    <col min="141" max="141" width="10.625" style="29"/>
-    <col min="142" max="142" width="10.625" style="11"/>
-    <col min="143" max="143" width="10.625" style="29"/>
-    <col min="144" max="144" width="10.625" style="11"/>
-    <col min="145" max="145" width="10.625" style="29"/>
-    <col min="146" max="146" width="10.625" style="11"/>
-    <col min="147" max="147" width="10.625" style="29"/>
-    <col min="148" max="148" width="10.625" style="11"/>
-    <col min="149" max="149" width="10.625" style="29"/>
-    <col min="150" max="153" width="10.625" style="11"/>
-    <col min="154" max="154" width="10.625" style="29"/>
-    <col min="155" max="155" width="10.625" style="11"/>
-    <col min="156" max="156" width="10.625" style="29"/>
-    <col min="157" max="161" width="10.625" style="11"/>
-    <col min="162" max="164" width="10.625" style="29"/>
-    <col min="165" max="166" width="10.625" style="11"/>
-    <col min="167" max="170" width="10.625" style="29"/>
-    <col min="171" max="171" width="10.625" style="11"/>
-    <col min="172" max="172" width="10.625" style="29"/>
-    <col min="173" max="175" width="10.625" style="11"/>
-    <col min="176" max="178" width="10.625" style="29"/>
-    <col min="179" max="179" width="10.625" style="11"/>
-    <col min="180" max="180" width="10.625" style="29"/>
-    <col min="181" max="16384" width="10.625" style="11"/>
+    <col min="1" max="11" width="10.5703125" style="11"/>
+    <col min="12" max="13" width="10.5703125" style="29"/>
+    <col min="14" max="14" width="10.5703125" style="11"/>
+    <col min="15" max="18" width="10.5703125" style="29"/>
+    <col min="19" max="20" width="10.5703125" style="11"/>
+    <col min="21" max="33" width="10.5703125" style="29"/>
+    <col min="34" max="34" width="10.5703125" style="11"/>
+    <col min="35" max="37" width="10.5703125" style="29"/>
+    <col min="38" max="38" width="10.5703125" style="11"/>
+    <col min="39" max="41" width="10.5703125" style="29"/>
+    <col min="42" max="43" width="10.5703125" style="11"/>
+    <col min="44" max="46" width="10.5703125" style="29"/>
+    <col min="47" max="51" width="10.5703125" style="11"/>
+    <col min="52" max="55" width="10.5703125" style="29"/>
+    <col min="56" max="60" width="10.5703125" style="11"/>
+    <col min="61" max="64" width="10.5703125" style="29"/>
+    <col min="65" max="69" width="10.5703125" style="11"/>
+    <col min="70" max="70" width="10.5703125" style="29"/>
+    <col min="71" max="72" width="10.5703125" style="11"/>
+    <col min="73" max="73" width="10.5703125" style="29"/>
+    <col min="74" max="74" width="10.5703125" style="11"/>
+    <col min="75" max="75" width="10.5703125" style="29"/>
+    <col min="76" max="76" width="10.5703125" style="11"/>
+    <col min="77" max="84" width="10.5703125" style="29"/>
+    <col min="85" max="88" width="10.5703125" style="11"/>
+    <col min="89" max="89" width="10.5703125" style="29"/>
+    <col min="90" max="90" width="10.5703125" style="11"/>
+    <col min="91" max="91" width="10.5703125" style="29"/>
+    <col min="92" max="92" width="10.5703125" style="11"/>
+    <col min="93" max="94" width="10.5703125" style="29"/>
+    <col min="95" max="95" width="10.5703125" style="11"/>
+    <col min="96" max="97" width="10.5703125" style="29"/>
+    <col min="98" max="98" width="10.5703125" style="11"/>
+    <col min="99" max="100" width="10.5703125" style="29"/>
+    <col min="101" max="103" width="10.5703125" style="11"/>
+    <col min="104" max="105" width="10.5703125" style="29"/>
+    <col min="106" max="108" width="10.5703125" style="11"/>
+    <col min="109" max="109" width="10.5703125" style="29"/>
+    <col min="110" max="110" width="10.5703125" style="11"/>
+    <col min="111" max="112" width="10.5703125" style="29"/>
+    <col min="113" max="116" width="10.5703125" style="11"/>
+    <col min="117" max="117" width="10.5703125" style="29"/>
+    <col min="118" max="119" width="10.5703125" style="11"/>
+    <col min="120" max="120" width="10.5703125" style="29"/>
+    <col min="121" max="122" width="10.5703125" style="11"/>
+    <col min="123" max="123" width="10.5703125" style="29"/>
+    <col min="124" max="125" width="10.5703125" style="11"/>
+    <col min="126" max="126" width="10.5703125" style="29"/>
+    <col min="127" max="128" width="10.5703125" style="11"/>
+    <col min="129" max="129" width="10.5703125" style="29"/>
+    <col min="130" max="131" width="10.5703125" style="11"/>
+    <col min="132" max="132" width="10.5703125" style="29"/>
+    <col min="133" max="134" width="10.5703125" style="11"/>
+    <col min="135" max="135" width="10.5703125" style="29"/>
+    <col min="136" max="137" width="10.5703125" style="11"/>
+    <col min="138" max="138" width="10.5703125" style="29"/>
+    <col min="139" max="140" width="10.5703125" style="11"/>
+    <col min="141" max="141" width="10.5703125" style="29"/>
+    <col min="142" max="142" width="10.5703125" style="11"/>
+    <col min="143" max="143" width="10.5703125" style="29"/>
+    <col min="144" max="144" width="10.5703125" style="11"/>
+    <col min="145" max="145" width="10.5703125" style="29"/>
+    <col min="146" max="146" width="10.5703125" style="11"/>
+    <col min="147" max="147" width="10.5703125" style="29"/>
+    <col min="148" max="148" width="10.5703125" style="11"/>
+    <col min="149" max="149" width="10.5703125" style="29"/>
+    <col min="150" max="153" width="10.5703125" style="11"/>
+    <col min="154" max="154" width="10.5703125" style="29"/>
+    <col min="155" max="155" width="10.5703125" style="11"/>
+    <col min="156" max="156" width="10.5703125" style="29"/>
+    <col min="157" max="161" width="10.5703125" style="11"/>
+    <col min="162" max="164" width="10.5703125" style="29"/>
+    <col min="165" max="166" width="10.5703125" style="11"/>
+    <col min="167" max="170" width="10.5703125" style="29"/>
+    <col min="171" max="171" width="10.5703125" style="11"/>
+    <col min="172" max="172" width="10.5703125" style="29"/>
+    <col min="173" max="175" width="10.5703125" style="11"/>
+    <col min="176" max="178" width="10.5703125" style="29"/>
+    <col min="179" max="179" width="10.5703125" style="11"/>
+    <col min="180" max="180" width="10.5703125" style="29"/>
+    <col min="181" max="16384" width="10.5703125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
@@ -5978,83 +5978,85 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EX26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="DQ1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="DV10" sqref="DV10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="10" width="10.625" style="11"/>
-    <col min="11" max="12" width="10.625" style="29"/>
-    <col min="13" max="13" width="10.625" style="11"/>
-    <col min="14" max="15" width="10.625" style="29"/>
-    <col min="16" max="17" width="10.625" style="11"/>
-    <col min="18" max="28" width="10.625" style="29"/>
-    <col min="29" max="31" width="10.625" style="11"/>
-    <col min="32" max="33" width="10.625" style="29"/>
-    <col min="34" max="36" width="10.625" style="11"/>
-    <col min="37" max="37" width="10.625" style="29"/>
-    <col min="38" max="39" width="10.625" style="11"/>
-    <col min="40" max="40" width="10.625" style="29"/>
-    <col min="41" max="41" width="10.625" style="11"/>
-    <col min="42" max="42" width="10.625" style="29"/>
-    <col min="43" max="43" width="10.625" style="11"/>
-    <col min="44" max="48" width="10.625" style="29"/>
-    <col min="49" max="52" width="10.625" style="11"/>
-    <col min="53" max="53" width="10.625" style="29"/>
-    <col min="54" max="54" width="10.625" style="11"/>
-    <col min="55" max="55" width="10.625" style="29"/>
-    <col min="56" max="57" width="10.625" style="11"/>
-    <col min="58" max="61" width="10.625" style="29"/>
-    <col min="62" max="63" width="10.625" style="11"/>
-    <col min="64" max="64" width="10.625" style="29"/>
-    <col min="65" max="74" width="10.625" style="11"/>
-    <col min="75" max="75" width="10.625" style="29"/>
-    <col min="76" max="78" width="10.625" style="11"/>
-    <col min="79" max="79" width="10.625" style="29"/>
-    <col min="80" max="83" width="10.625" style="11"/>
-    <col min="84" max="85" width="10.625" style="29"/>
-    <col min="86" max="88" width="10.625" style="11"/>
-    <col min="89" max="89" width="10.625" style="29"/>
-    <col min="90" max="91" width="10.625" style="11"/>
-    <col min="92" max="92" width="10.625" style="29"/>
-    <col min="93" max="94" width="10.625" style="11"/>
-    <col min="95" max="95" width="10.625" style="29"/>
-    <col min="96" max="97" width="10.625" style="11"/>
-    <col min="98" max="98" width="10.625" style="29"/>
-    <col min="99" max="100" width="10.625" style="11"/>
-    <col min="101" max="101" width="10.625" style="29"/>
-    <col min="102" max="103" width="10.625" style="11"/>
-    <col min="104" max="104" width="10.625" style="29"/>
-    <col min="105" max="106" width="10.625" style="11"/>
-    <col min="107" max="107" width="10.625" style="29"/>
-    <col min="108" max="109" width="10.625" style="11"/>
-    <col min="110" max="110" width="10.625" style="29"/>
-    <col min="111" max="112" width="10.625" style="11"/>
-    <col min="113" max="113" width="10.625" style="29"/>
-    <col min="114" max="114" width="10.625" style="11"/>
-    <col min="115" max="115" width="10.625" style="29"/>
-    <col min="116" max="116" width="10.625" style="11"/>
-    <col min="117" max="117" width="10.625" style="29"/>
-    <col min="118" max="118" width="10.625" style="11"/>
-    <col min="119" max="119" width="10.625" style="29"/>
-    <col min="120" max="120" width="10.625" style="11"/>
-    <col min="121" max="121" width="10.625" style="29"/>
-    <col min="122" max="124" width="10.625" style="11"/>
-    <col min="125" max="125" width="10.625" style="29"/>
-    <col min="126" max="126" width="10.625" style="11"/>
-    <col min="127" max="127" width="10.625" style="29"/>
-    <col min="128" max="128" width="10.625" style="11"/>
-    <col min="129" max="129" width="10.625" style="29"/>
-    <col min="130" max="132" width="10.625" style="11"/>
-    <col min="133" max="135" width="10.625" style="29"/>
-    <col min="136" max="137" width="10.625" style="11"/>
-    <col min="138" max="141" width="10.625" style="29"/>
-    <col min="142" max="142" width="10.625" style="11"/>
-    <col min="143" max="143" width="10.625" style="29"/>
-    <col min="144" max="146" width="10.625" style="11"/>
-    <col min="147" max="149" width="10.625" style="29"/>
-    <col min="150" max="150" width="10.625" style="11"/>
-    <col min="151" max="151" width="10.625" style="29"/>
-    <col min="152" max="16384" width="10.625" style="11"/>
+    <col min="1" max="10" width="10.5703125" style="11"/>
+    <col min="11" max="12" width="10.5703125" style="29"/>
+    <col min="13" max="13" width="10.5703125" style="11"/>
+    <col min="14" max="15" width="10.5703125" style="29"/>
+    <col min="16" max="17" width="10.5703125" style="11"/>
+    <col min="18" max="28" width="10.5703125" style="29"/>
+    <col min="29" max="31" width="10.5703125" style="11"/>
+    <col min="32" max="33" width="10.5703125" style="29"/>
+    <col min="34" max="36" width="10.5703125" style="11"/>
+    <col min="37" max="37" width="10.5703125" style="29"/>
+    <col min="38" max="39" width="10.5703125" style="11"/>
+    <col min="40" max="40" width="10.5703125" style="29"/>
+    <col min="41" max="41" width="10.5703125" style="11"/>
+    <col min="42" max="42" width="10.5703125" style="29"/>
+    <col min="43" max="43" width="10.5703125" style="11"/>
+    <col min="44" max="48" width="10.5703125" style="29"/>
+    <col min="49" max="52" width="10.5703125" style="11"/>
+    <col min="53" max="53" width="10.5703125" style="29"/>
+    <col min="54" max="54" width="10.5703125" style="11"/>
+    <col min="55" max="55" width="10.5703125" style="29"/>
+    <col min="56" max="57" width="10.5703125" style="11"/>
+    <col min="58" max="61" width="10.5703125" style="29"/>
+    <col min="62" max="63" width="10.5703125" style="11"/>
+    <col min="64" max="64" width="10.5703125" style="29"/>
+    <col min="65" max="74" width="10.5703125" style="11"/>
+    <col min="75" max="75" width="10.5703125" style="29"/>
+    <col min="76" max="78" width="10.5703125" style="11"/>
+    <col min="79" max="79" width="10.5703125" style="29"/>
+    <col min="80" max="83" width="10.5703125" style="11"/>
+    <col min="84" max="85" width="10.5703125" style="29"/>
+    <col min="86" max="88" width="10.5703125" style="11"/>
+    <col min="89" max="89" width="10.5703125" style="29"/>
+    <col min="90" max="91" width="10.5703125" style="11"/>
+    <col min="92" max="92" width="10.5703125" style="29"/>
+    <col min="93" max="94" width="10.5703125" style="11"/>
+    <col min="95" max="95" width="10.5703125" style="29"/>
+    <col min="96" max="97" width="10.5703125" style="11"/>
+    <col min="98" max="98" width="10.5703125" style="29"/>
+    <col min="99" max="100" width="10.5703125" style="11"/>
+    <col min="101" max="101" width="10.5703125" style="29"/>
+    <col min="102" max="103" width="10.5703125" style="11"/>
+    <col min="104" max="104" width="10.5703125" style="29"/>
+    <col min="105" max="106" width="10.5703125" style="11"/>
+    <col min="107" max="107" width="10.5703125" style="29"/>
+    <col min="108" max="109" width="10.5703125" style="11"/>
+    <col min="110" max="110" width="10.5703125" style="29"/>
+    <col min="111" max="112" width="10.5703125" style="11"/>
+    <col min="113" max="113" width="10.5703125" style="29"/>
+    <col min="114" max="114" width="10.5703125" style="11"/>
+    <col min="115" max="115" width="10.5703125" style="29"/>
+    <col min="116" max="116" width="10.5703125" style="11"/>
+    <col min="117" max="117" width="10.5703125" style="29"/>
+    <col min="118" max="118" width="10.5703125" style="11"/>
+    <col min="119" max="119" width="10.5703125" style="29"/>
+    <col min="120" max="120" width="10.5703125" style="11"/>
+    <col min="121" max="121" width="10.5703125" style="29"/>
+    <col min="122" max="124" width="10.5703125" style="11"/>
+    <col min="125" max="125" width="10.5703125" style="29"/>
+    <col min="126" max="126" width="10.5703125" style="11"/>
+    <col min="127" max="127" width="10.5703125" style="29"/>
+    <col min="128" max="128" width="10.5703125" style="11"/>
+    <col min="129" max="129" width="10.5703125" style="29"/>
+    <col min="130" max="132" width="10.5703125" style="11"/>
+    <col min="133" max="135" width="10.5703125" style="29"/>
+    <col min="136" max="137" width="10.5703125" style="11"/>
+    <col min="138" max="141" width="10.5703125" style="29"/>
+    <col min="142" max="142" width="10.5703125" style="11"/>
+    <col min="143" max="143" width="10.5703125" style="29"/>
+    <col min="144" max="146" width="10.5703125" style="11"/>
+    <col min="147" max="149" width="10.5703125" style="29"/>
+    <col min="150" max="150" width="10.5703125" style="11"/>
+    <col min="151" max="151" width="10.5703125" style="29"/>
+    <col min="152" max="16384" width="10.5703125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
@@ -7703,7 +7705,7 @@
       <c r="DV11" s="4"/>
       <c r="DW11" s="15"/>
       <c r="DX11" s="4"/>
-      <c r="DY11" s="15"/>
+      <c r="DY11" s="36"/>
       <c r="DZ11" s="4"/>
       <c r="EA11" s="4"/>
       <c r="EB11" s="4"/>
@@ -7859,7 +7861,7 @@
       <c r="DV12" s="9"/>
       <c r="DW12" s="17"/>
       <c r="DX12" s="9"/>
-      <c r="DY12" s="17"/>
+      <c r="DY12" s="9"/>
       <c r="DZ12" s="9"/>
       <c r="EA12" s="9"/>
       <c r="EB12" s="9"/>
@@ -8015,7 +8017,7 @@
       <c r="DV13" s="9"/>
       <c r="DW13" s="17"/>
       <c r="DX13" s="9"/>
-      <c r="DY13" s="17"/>
+      <c r="DY13" s="9"/>
       <c r="DZ13" s="9"/>
       <c r="EA13" s="9"/>
       <c r="EB13" s="9"/>
@@ -8171,7 +8173,7 @@
       <c r="DV14" s="10"/>
       <c r="DW14" s="18"/>
       <c r="DX14" s="10"/>
-      <c r="DY14" s="18"/>
+      <c r="DY14" s="10"/>
       <c r="DZ14" s="10"/>
       <c r="EA14" s="10"/>
       <c r="EB14" s="10"/>
@@ -8327,7 +8329,7 @@
       <c r="DV15" s="10"/>
       <c r="DW15" s="18"/>
       <c r="DX15" s="10"/>
-      <c r="DY15" s="18"/>
+      <c r="DY15" s="10"/>
       <c r="DZ15" s="10"/>
       <c r="EA15" s="10"/>
       <c r="EB15" s="10"/>
@@ -8483,7 +8485,7 @@
       <c r="DV16" s="10"/>
       <c r="DW16" s="18"/>
       <c r="DX16" s="10"/>
-      <c r="DY16" s="18"/>
+      <c r="DY16" s="10"/>
       <c r="DZ16" s="10"/>
       <c r="EA16" s="10"/>
       <c r="EB16" s="10"/>
@@ -8643,7 +8645,7 @@
       <c r="DV17" s="10"/>
       <c r="DW17" s="18"/>
       <c r="DX17" s="10"/>
-      <c r="DY17" s="18"/>
+      <c r="DY17" s="10"/>
       <c r="DZ17" s="10"/>
       <c r="EA17" s="10"/>
       <c r="EB17" s="10"/>
@@ -8807,7 +8809,7 @@
       <c r="DV18" s="10"/>
       <c r="DW18" s="18"/>
       <c r="DX18" s="10"/>
-      <c r="DY18" s="18"/>
+      <c r="DY18" s="10"/>
       <c r="DZ18" s="10"/>
       <c r="EA18" s="10"/>
       <c r="EB18" s="10"/>
@@ -8963,7 +8965,7 @@
       <c r="DV19" s="10"/>
       <c r="DW19" s="18"/>
       <c r="DX19" s="10"/>
-      <c r="DY19" s="18"/>
+      <c r="DY19" s="10"/>
       <c r="DZ19" s="10"/>
       <c r="EA19" s="10"/>
       <c r="EB19" s="10"/>
@@ -9119,7 +9121,7 @@
       <c r="DV20" s="13"/>
       <c r="DW20" s="22"/>
       <c r="DX20" s="13"/>
-      <c r="DY20" s="22"/>
+      <c r="DY20" s="13"/>
       <c r="DZ20" s="13"/>
       <c r="EA20" s="13"/>
       <c r="EB20" s="13"/>
@@ -9197,85 +9199,87 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:GC20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="ES1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="FA25" sqref="FA25"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
+  <sheetFormatPr defaultColWidth="10.5703125" defaultRowHeight="12" customHeight="1"/>
   <cols>
-    <col min="1" max="10" width="10.625" style="11"/>
-    <col min="11" max="12" width="10.625" style="29"/>
-    <col min="13" max="13" width="10.625" style="11"/>
-    <col min="14" max="15" width="10.625" style="29"/>
-    <col min="16" max="19" width="10.625" style="11"/>
-    <col min="20" max="31" width="10.625" style="29"/>
-    <col min="32" max="32" width="10.625" style="11"/>
-    <col min="33" max="35" width="10.625" style="29"/>
-    <col min="36" max="36" width="10.625" style="11"/>
-    <col min="37" max="39" width="10.625" style="29"/>
-    <col min="40" max="40" width="10.625" style="11"/>
-    <col min="41" max="43" width="10.625" style="29"/>
-    <col min="44" max="46" width="10.625" style="11"/>
-    <col min="47" max="49" width="10.625" style="29"/>
-    <col min="50" max="52" width="10.625" style="11"/>
-    <col min="53" max="55" width="10.625" style="29"/>
-    <col min="56" max="60" width="10.625" style="11"/>
-    <col min="61" max="61" width="10.625" style="29"/>
-    <col min="62" max="62" width="10.625" style="11"/>
-    <col min="63" max="63" width="10.625" style="29"/>
-    <col min="64" max="64" width="10.625" style="11"/>
-    <col min="65" max="66" width="10.625" style="29"/>
-    <col min="67" max="68" width="10.625" style="11"/>
-    <col min="69" max="70" width="10.625" style="29"/>
-    <col min="71" max="76" width="10.625" style="11"/>
-    <col min="77" max="77" width="10.625" style="29"/>
-    <col min="78" max="78" width="10.625" style="11"/>
-    <col min="79" max="79" width="10.625" style="29"/>
-    <col min="80" max="81" width="10.625" style="11"/>
-    <col min="82" max="93" width="10.625" style="29"/>
-    <col min="94" max="103" width="10.625" style="11"/>
-    <col min="104" max="105" width="10.625" style="29"/>
-    <col min="106" max="108" width="10.625" style="11"/>
-    <col min="109" max="109" width="10.625" style="29"/>
-    <col min="110" max="111" width="10.625" style="11"/>
-    <col min="112" max="115" width="10.625" style="29"/>
-    <col min="116" max="118" width="10.625" style="11"/>
-    <col min="119" max="119" width="10.625" style="29"/>
-    <col min="120" max="121" width="10.625" style="11"/>
-    <col min="122" max="122" width="10.625" style="29"/>
-    <col min="123" max="124" width="10.625" style="11"/>
-    <col min="125" max="125" width="10.625" style="29"/>
-    <col min="126" max="127" width="10.625" style="11"/>
-    <col min="128" max="128" width="10.625" style="29"/>
-    <col min="129" max="130" width="10.625" style="11"/>
-    <col min="131" max="131" width="10.625" style="29"/>
-    <col min="132" max="133" width="10.625" style="11"/>
-    <col min="134" max="134" width="10.625" style="29"/>
-    <col min="135" max="136" width="10.625" style="11"/>
-    <col min="137" max="137" width="10.625" style="29"/>
-    <col min="138" max="139" width="10.625" style="11"/>
-    <col min="140" max="140" width="10.625" style="29"/>
-    <col min="141" max="142" width="10.625" style="11"/>
-    <col min="143" max="143" width="10.625" style="29"/>
-    <col min="144" max="144" width="10.625" style="11"/>
-    <col min="145" max="145" width="10.625" style="29"/>
-    <col min="146" max="146" width="10.625" style="11"/>
-    <col min="147" max="147" width="10.625" style="29"/>
-    <col min="148" max="148" width="10.625" style="11"/>
-    <col min="149" max="149" width="10.625" style="29"/>
-    <col min="150" max="150" width="10.625" style="11"/>
-    <col min="151" max="151" width="10.625" style="29"/>
-    <col min="152" max="155" width="10.625" style="11"/>
-    <col min="156" max="157" width="10.625" style="29"/>
-    <col min="158" max="163" width="10.625" style="11"/>
-    <col min="164" max="166" width="10.625" style="29"/>
-    <col min="167" max="168" width="10.625" style="11"/>
-    <col min="169" max="172" width="10.625" style="29"/>
-    <col min="173" max="173" width="10.625" style="11"/>
-    <col min="174" max="174" width="10.625" style="29"/>
-    <col min="175" max="177" width="10.625" style="11"/>
-    <col min="178" max="180" width="10.625" style="29"/>
-    <col min="181" max="181" width="10.625" style="11"/>
-    <col min="182" max="182" width="10.625" style="29"/>
-    <col min="183" max="16384" width="10.625" style="11"/>
+    <col min="1" max="10" width="10.5703125" style="11"/>
+    <col min="11" max="12" width="10.5703125" style="29"/>
+    <col min="13" max="13" width="10.5703125" style="11"/>
+    <col min="14" max="15" width="10.5703125" style="29"/>
+    <col min="16" max="19" width="10.5703125" style="11"/>
+    <col min="20" max="31" width="10.5703125" style="29"/>
+    <col min="32" max="32" width="10.5703125" style="11"/>
+    <col min="33" max="35" width="10.5703125" style="29"/>
+    <col min="36" max="36" width="10.5703125" style="11"/>
+    <col min="37" max="39" width="10.5703125" style="29"/>
+    <col min="40" max="40" width="10.5703125" style="11"/>
+    <col min="41" max="43" width="10.5703125" style="29"/>
+    <col min="44" max="46" width="10.5703125" style="11"/>
+    <col min="47" max="49" width="10.5703125" style="29"/>
+    <col min="50" max="52" width="10.5703125" style="11"/>
+    <col min="53" max="55" width="10.5703125" style="29"/>
+    <col min="56" max="60" width="10.5703125" style="11"/>
+    <col min="61" max="61" width="10.5703125" style="29"/>
+    <col min="62" max="62" width="10.5703125" style="11"/>
+    <col min="63" max="63" width="10.5703125" style="29"/>
+    <col min="64" max="64" width="10.5703125" style="11"/>
+    <col min="65" max="66" width="10.5703125" style="29"/>
+    <col min="67" max="68" width="10.5703125" style="11"/>
+    <col min="69" max="70" width="10.5703125" style="29"/>
+    <col min="71" max="76" width="10.5703125" style="11"/>
+    <col min="77" max="77" width="10.5703125" style="29"/>
+    <col min="78" max="78" width="10.5703125" style="11"/>
+    <col min="79" max="79" width="10.5703125" style="29"/>
+    <col min="80" max="81" width="10.5703125" style="11"/>
+    <col min="82" max="93" width="10.5703125" style="29"/>
+    <col min="94" max="103" width="10.5703125" style="11"/>
+    <col min="104" max="105" width="10.5703125" style="29"/>
+    <col min="106" max="108" width="10.5703125" style="11"/>
+    <col min="109" max="109" width="10.5703125" style="29"/>
+    <col min="110" max="111" width="10.5703125" style="11"/>
+    <col min="112" max="115" width="10.5703125" style="29"/>
+    <col min="116" max="118" width="10.5703125" style="11"/>
+    <col min="119" max="119" width="10.5703125" style="29"/>
+    <col min="120" max="121" width="10.5703125" style="11"/>
+    <col min="122" max="122" width="10.5703125" style="29"/>
+    <col min="123" max="124" width="10.5703125" style="11"/>
+    <col min="125" max="125" width="10.5703125" style="29"/>
+    <col min="126" max="127" width="10.5703125" style="11"/>
+    <col min="128" max="128" width="10.5703125" style="29"/>
+    <col min="129" max="130" width="10.5703125" style="11"/>
+    <col min="131" max="131" width="10.5703125" style="29"/>
+    <col min="132" max="133" width="10.5703125" style="11"/>
+    <col min="134" max="134" width="10.5703125" style="29"/>
+    <col min="135" max="136" width="10.5703125" style="11"/>
+    <col min="137" max="137" width="10.5703125" style="29"/>
+    <col min="138" max="139" width="10.5703125" style="11"/>
+    <col min="140" max="140" width="10.5703125" style="29"/>
+    <col min="141" max="142" width="10.5703125" style="11"/>
+    <col min="143" max="143" width="10.5703125" style="29"/>
+    <col min="144" max="144" width="10.5703125" style="11"/>
+    <col min="145" max="145" width="10.5703125" style="29"/>
+    <col min="146" max="146" width="10.5703125" style="11"/>
+    <col min="147" max="147" width="10.5703125" style="29"/>
+    <col min="148" max="148" width="10.5703125" style="11"/>
+    <col min="149" max="149" width="10.5703125" style="29"/>
+    <col min="150" max="150" width="10.5703125" style="11"/>
+    <col min="151" max="151" width="10.5703125" style="29"/>
+    <col min="152" max="155" width="10.5703125" style="11"/>
+    <col min="156" max="157" width="10.5703125" style="29"/>
+    <col min="158" max="163" width="10.5703125" style="11"/>
+    <col min="164" max="166" width="10.5703125" style="29"/>
+    <col min="167" max="168" width="10.5703125" style="11"/>
+    <col min="169" max="172" width="10.5703125" style="29"/>
+    <col min="173" max="173" width="10.5703125" style="11"/>
+    <col min="174" max="174" width="10.5703125" style="29"/>
+    <col min="175" max="177" width="10.5703125" style="11"/>
+    <col min="178" max="180" width="10.5703125" style="29"/>
+    <col min="181" max="181" width="10.5703125" style="11"/>
+    <col min="182" max="182" width="10.5703125" style="29"/>
+    <col min="183" max="16384" width="10.5703125" style="11"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
@@ -11263,7 +11267,7 @@
       <c r="EX11" s="4"/>
       <c r="EY11" s="4"/>
       <c r="EZ11" s="15"/>
-      <c r="FA11" s="15"/>
+      <c r="FA11" s="36"/>
       <c r="FB11" s="4"/>
       <c r="FC11" s="4"/>
       <c r="FD11" s="4"/>
@@ -11449,7 +11453,7 @@
       <c r="EX12" s="9"/>
       <c r="EY12" s="9"/>
       <c r="EZ12" s="17"/>
-      <c r="FA12" s="17"/>
+      <c r="FA12" s="9"/>
       <c r="FB12" s="9"/>
       <c r="FC12" s="9"/>
       <c r="FD12" s="9"/>
@@ -11636,7 +11640,7 @@
       <c r="EX13" s="10"/>
       <c r="EY13" s="10"/>
       <c r="EZ13" s="18"/>
-      <c r="FA13" s="18"/>
+      <c r="FA13" s="10"/>
       <c r="FB13" s="10"/>
       <c r="FC13" s="10"/>
       <c r="FD13" s="10"/>
@@ -11823,7 +11827,7 @@
       <c r="EX14" s="10"/>
       <c r="EY14" s="10"/>
       <c r="EZ14" s="18"/>
-      <c r="FA14" s="18"/>
+      <c r="FA14" s="10"/>
       <c r="FB14" s="10"/>
       <c r="FC14" s="10"/>
       <c r="FD14" s="10"/>
@@ -12010,7 +12014,7 @@
       <c r="EX15" s="10"/>
       <c r="EY15" s="10"/>
       <c r="EZ15" s="18"/>
-      <c r="FA15" s="18"/>
+      <c r="FA15" s="10"/>
       <c r="FB15" s="10"/>
       <c r="FC15" s="10"/>
       <c r="FD15" s="10"/>
@@ -12197,7 +12201,7 @@
       <c r="EX16" s="10"/>
       <c r="EY16" s="10"/>
       <c r="EZ16" s="18"/>
-      <c r="FA16" s="18"/>
+      <c r="FA16" s="10"/>
       <c r="FB16" s="10"/>
       <c r="FC16" s="10"/>
       <c r="FD16" s="10"/>
@@ -12392,7 +12396,7 @@
       <c r="EX17" s="10"/>
       <c r="EY17" s="10"/>
       <c r="EZ17" s="18"/>
-      <c r="FA17" s="18"/>
+      <c r="FA17" s="10"/>
       <c r="FB17" s="10"/>
       <c r="FC17" s="10"/>
       <c r="FD17" s="10"/>
@@ -12595,7 +12599,7 @@
       <c r="EX18" s="10"/>
       <c r="EY18" s="10"/>
       <c r="EZ18" s="18"/>
-      <c r="FA18" s="18"/>
+      <c r="FA18" s="10"/>
       <c r="FB18" s="10"/>
       <c r="FC18" s="10"/>
       <c r="FD18" s="10"/>
@@ -12782,7 +12786,7 @@
       <c r="EX19" s="10"/>
       <c r="EY19" s="10"/>
       <c r="EZ19" s="18"/>
-      <c r="FA19" s="18"/>
+      <c r="FA19" s="10"/>
       <c r="FB19" s="10"/>
       <c r="FC19" s="10"/>
       <c r="FD19" s="10"/>
@@ -12969,7 +12973,7 @@
       <c r="EX20" s="13"/>
       <c r="EY20" s="13"/>
       <c r="EZ20" s="22"/>
-      <c r="FA20" s="22"/>
+      <c r="FA20" s="13"/>
       <c r="FB20" s="13"/>
       <c r="FC20" s="13"/>
       <c r="FD20" s="13"/>

</xml_diff>

<commit_message>
update code: Multi language KMK003
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="724" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="730" uniqueCount="190">
   <si>
     <t>コード</t>
   </si>
@@ -1122,6 +1122,29 @@
   </si>
   <si>
     <t>流動休憩設定 外出を休憩として扱う</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>他言語名称</t>
+    <rPh sb="0" eb="3">
+      <t>タゲンゴ</t>
+    </rPh>
+    <rPh sb="3" eb="5">
+      <t>メイショウ</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>他言語略名</t>
+    <rPh sb="0" eb="3">
+      <t>タゲンゴ</t>
+    </rPh>
+    <rPh sb="3" eb="4">
+      <t>リャク</t>
+    </rPh>
+    <rPh sb="4" eb="5">
+      <t>メイ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1596,7 +1619,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="標準" xfId="0" builtinId="0"/>
     <cellStyle name="標準 2" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1951,9 +1974,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GF20"/>
+  <dimension ref="A1:GH20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="FI1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="GG10" sqref="GG10:GH20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
   <cols>
@@ -2040,7 +2065,7 @@
     <col min="181" max="16384" width="10.625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="1" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
@@ -2164,7 +2189,7 @@
       <c r="FV1" s="27"/>
       <c r="FX1" s="27"/>
     </row>
-    <row r="2" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="2" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -2288,7 +2313,7 @@
       <c r="FV2" s="27"/>
       <c r="FX2" s="27"/>
     </row>
-    <row r="3" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="3" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -2412,7 +2437,7 @@
       <c r="FV3" s="27"/>
       <c r="FX3" s="27"/>
     </row>
-    <row r="4" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>158</v>
       </c>
@@ -2536,7 +2561,7 @@
       <c r="FV4" s="27"/>
       <c r="FX4" s="27"/>
     </row>
-    <row r="5" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A5"/>
       <c r="B5"/>
       <c r="C5"/>
@@ -2726,7 +2751,7 @@
       <c r="GE5"/>
       <c r="GF5"/>
     </row>
-    <row r="6" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="6" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -2916,7 +2941,7 @@
       <c r="GE6"/>
       <c r="GF6"/>
     </row>
-    <row r="7" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="7" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="L7" s="27"/>
       <c r="M7" s="27"/>
       <c r="O7" s="27"/>
@@ -3005,7 +3030,7 @@
       <c r="FV7" s="27"/>
       <c r="FX7" s="27"/>
     </row>
-    <row r="8" spans="1:188" s="43" customFormat="1">
+    <row r="8" spans="1:190" s="43" customFormat="1">
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -3232,7 +3257,7 @@
       <c r="GE8" s="46"/>
       <c r="GF8" s="47"/>
     </row>
-    <row r="9" spans="1:188" s="43" customFormat="1">
+    <row r="9" spans="1:190" s="43" customFormat="1">
       <c r="A9" s="67"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
@@ -3504,7 +3529,7 @@
       <c r="GE9" s="46"/>
       <c r="GF9" s="47"/>
     </row>
-    <row r="10" spans="1:188" s="43" customFormat="1" ht="12" customHeight="1">
+    <row r="10" spans="1:190" s="43" customFormat="1" ht="12" customHeight="1">
       <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
@@ -4061,8 +4086,14 @@
       <c r="GF10" s="66" t="s">
         <v>123</v>
       </c>
+      <c r="GG10" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="GH10" s="65" t="s">
+        <v>189</v>
+      </c>
     </row>
-    <row r="11" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -4251,8 +4282,10 @@
       <c r="GD11" s="4"/>
       <c r="GE11" s="4"/>
       <c r="GF11" s="36"/>
+      <c r="GG11" s="36"/>
+      <c r="GH11" s="36"/>
     </row>
-    <row r="12" spans="1:188" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="12" spans="1:190" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -4441,8 +4474,10 @@
       <c r="GD12" s="9"/>
       <c r="GE12" s="9"/>
       <c r="GF12" s="9"/>
+      <c r="GG12" s="9"/>
+      <c r="GH12" s="9"/>
     </row>
-    <row r="13" spans="1:188" ht="12" customHeight="1">
+    <row r="13" spans="1:190" ht="12" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -4631,8 +4666,10 @@
       <c r="GD13" s="10"/>
       <c r="GE13" s="10"/>
       <c r="GF13" s="10"/>
+      <c r="GG13" s="10"/>
+      <c r="GH13" s="10"/>
     </row>
-    <row r="14" spans="1:188" ht="12" customHeight="1">
+    <row r="14" spans="1:190" ht="12" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -4821,8 +4858,10 @@
       <c r="GD14" s="10"/>
       <c r="GE14" s="10"/>
       <c r="GF14" s="10"/>
+      <c r="GG14" s="10"/>
+      <c r="GH14" s="10"/>
     </row>
-    <row r="15" spans="1:188" ht="12" customHeight="1">
+    <row r="15" spans="1:190" ht="12" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -5011,8 +5050,10 @@
       <c r="GD15" s="10"/>
       <c r="GE15" s="10"/>
       <c r="GF15" s="10"/>
+      <c r="GG15" s="10"/>
+      <c r="GH15" s="10"/>
     </row>
-    <row r="16" spans="1:188" ht="12" customHeight="1">
+    <row r="16" spans="1:190" ht="12" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -5201,8 +5242,10 @@
       <c r="GD16" s="10"/>
       <c r="GE16" s="10"/>
       <c r="GF16" s="10"/>
+      <c r="GG16" s="10"/>
+      <c r="GH16" s="10"/>
     </row>
-    <row r="17" spans="1:188" ht="12" customHeight="1">
+    <row r="17" spans="1:190" ht="12" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -5391,8 +5434,10 @@
       <c r="GD17" s="10"/>
       <c r="GE17" s="10"/>
       <c r="GF17" s="10"/>
+      <c r="GG17" s="10"/>
+      <c r="GH17" s="10"/>
     </row>
-    <row r="18" spans="1:188" ht="12" customHeight="1">
+    <row r="18" spans="1:190" ht="12" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -5581,8 +5626,10 @@
       <c r="GD18" s="10"/>
       <c r="GE18" s="10"/>
       <c r="GF18" s="10"/>
+      <c r="GG18" s="10"/>
+      <c r="GH18" s="10"/>
     </row>
-    <row r="19" spans="1:188" ht="12" customHeight="1">
+    <row r="19" spans="1:190" ht="12" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -5771,8 +5818,10 @@
       <c r="GD19" s="10"/>
       <c r="GE19" s="10"/>
       <c r="GF19" s="10"/>
+      <c r="GG19" s="10"/>
+      <c r="GH19" s="10"/>
     </row>
-    <row r="20" spans="1:188" ht="12" customHeight="1">
+    <row r="20" spans="1:190" ht="12" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -5961,6 +6010,8 @@
       <c r="GD20" s="13"/>
       <c r="GE20" s="13"/>
       <c r="GF20" s="13"/>
+      <c r="GG20" s="13"/>
+      <c r="GH20" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -5976,9 +6027,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:EX26"/>
+  <dimension ref="A1:EZ26"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" topLeftCell="EE1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="EY10" sqref="EY10:EZ20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
   <cols>
@@ -6057,7 +6110,7 @@
     <col min="152" max="16384" width="10.625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="1" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
@@ -6145,7 +6198,7 @@
       <c r="ES1" s="27"/>
       <c r="EU1" s="27"/>
     </row>
-    <row r="2" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="2" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -6233,7 +6286,7 @@
       <c r="ES2" s="27"/>
       <c r="EU2" s="27"/>
     </row>
-    <row r="3" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="3" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -6321,7 +6374,7 @@
       <c r="ES3" s="27"/>
       <c r="EU3" s="27"/>
     </row>
-    <row r="4" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>158</v>
       </c>
@@ -6409,7 +6462,7 @@
       <c r="ES4" s="27"/>
       <c r="EU4" s="27"/>
     </row>
-    <row r="5" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="N5" s="27"/>
@@ -6475,7 +6528,7 @@
       <c r="ES5" s="27"/>
       <c r="EU5" s="27"/>
     </row>
-    <row r="6" spans="1:154" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="6" spans="1:156" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A6" s="33"/>
       <c r="B6" s="33"/>
       <c r="C6" s="33"/>
@@ -6631,7 +6684,7 @@
       <c r="EW6" s="33"/>
       <c r="EX6" s="33"/>
     </row>
-    <row r="7" spans="1:154" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="7" spans="1:156" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="H7" s="2"/>
       <c r="K7" s="32"/>
       <c r="L7" s="32"/>
@@ -6699,7 +6752,7 @@
       <c r="ES7" s="32"/>
       <c r="EU7" s="32"/>
     </row>
-    <row r="8" spans="1:154" s="43" customFormat="1">
+    <row r="8" spans="1:156" s="43" customFormat="1">
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -6892,7 +6945,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:154" s="43" customFormat="1">
+    <row r="9" spans="1:156" s="43" customFormat="1">
       <c r="A9" s="67"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
@@ -7116,7 +7169,7 @@
       <c r="EW9" s="62"/>
       <c r="EX9" s="68"/>
     </row>
-    <row r="10" spans="1:154" s="43" customFormat="1">
+    <row r="10" spans="1:156" s="43" customFormat="1">
       <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
@@ -7573,8 +7626,14 @@
       <c r="EX10" s="66" t="s">
         <v>119</v>
       </c>
+      <c r="EY10" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="EZ10" s="65" t="s">
+        <v>189</v>
+      </c>
     </row>
-    <row r="11" spans="1:154" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:156" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -7729,8 +7788,10 @@
       <c r="EV11" s="4"/>
       <c r="EW11" s="4"/>
       <c r="EX11" s="4"/>
+      <c r="EY11" s="36"/>
+      <c r="EZ11" s="36"/>
     </row>
-    <row r="12" spans="1:154" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="12" spans="1:156" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -7885,8 +7946,10 @@
       <c r="EV12" s="9"/>
       <c r="EW12" s="9"/>
       <c r="EX12" s="9"/>
+      <c r="EY12" s="9"/>
+      <c r="EZ12" s="9"/>
     </row>
-    <row r="13" spans="1:154" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="13" spans="1:156" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="9"/>
       <c r="B13" s="9"/>
       <c r="C13" s="9"/>
@@ -8041,8 +8104,10 @@
       <c r="EV13" s="9"/>
       <c r="EW13" s="9"/>
       <c r="EX13" s="9"/>
+      <c r="EY13" s="10"/>
+      <c r="EZ13" s="10"/>
     </row>
-    <row r="14" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="14" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -8197,8 +8262,10 @@
       <c r="EV14" s="10"/>
       <c r="EW14" s="10"/>
       <c r="EX14" s="10"/>
+      <c r="EY14" s="10"/>
+      <c r="EZ14" s="10"/>
     </row>
-    <row r="15" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="15" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -8353,8 +8420,10 @@
       <c r="EV15" s="10"/>
       <c r="EW15" s="10"/>
       <c r="EX15" s="10"/>
+      <c r="EY15" s="10"/>
+      <c r="EZ15" s="10"/>
     </row>
-    <row r="16" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="16" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -8509,8 +8578,10 @@
       <c r="EV16" s="10"/>
       <c r="EW16" s="10"/>
       <c r="EX16" s="10"/>
+      <c r="EY16" s="10"/>
+      <c r="EZ16" s="10"/>
     </row>
-    <row r="17" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="17" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -8669,8 +8740,10 @@
       <c r="EV17" s="10"/>
       <c r="EW17" s="10"/>
       <c r="EX17" s="10"/>
+      <c r="EY17" s="10"/>
+      <c r="EZ17" s="10"/>
     </row>
-    <row r="18" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="18" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -8833,8 +8906,10 @@
       <c r="EV18" s="10"/>
       <c r="EW18" s="10"/>
       <c r="EX18" s="10"/>
+      <c r="EY18" s="10"/>
+      <c r="EZ18" s="10"/>
     </row>
-    <row r="19" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="19" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -8989,8 +9064,10 @@
       <c r="EV19" s="10"/>
       <c r="EW19" s="10"/>
       <c r="EX19" s="10"/>
+      <c r="EY19" s="10"/>
+      <c r="EZ19" s="10"/>
     </row>
-    <row r="20" spans="1:154" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="20" spans="1:156" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -9145,38 +9222,40 @@
       <c r="EV20" s="13"/>
       <c r="EW20" s="13"/>
       <c r="EX20" s="13"/>
+      <c r="EY20" s="13"/>
+      <c r="EZ20" s="13"/>
     </row>
-    <row r="21" spans="1:154" ht="12" customHeight="1">
+    <row r="21" spans="1:156" ht="12" customHeight="1">
       <c r="DO21" s="35"/>
       <c r="DP21" s="24"/>
       <c r="DQ21" s="35"/>
       <c r="DR21" s="24"/>
     </row>
-    <row r="22" spans="1:154" ht="12" customHeight="1">
+    <row r="22" spans="1:156" ht="12" customHeight="1">
       <c r="DO22" s="35"/>
       <c r="DP22" s="24"/>
       <c r="DQ22" s="35"/>
       <c r="DR22" s="24"/>
     </row>
-    <row r="23" spans="1:154" ht="12" customHeight="1">
+    <row r="23" spans="1:156" ht="12" customHeight="1">
       <c r="DO23" s="35"/>
       <c r="DP23" s="24"/>
       <c r="DQ23" s="35"/>
       <c r="DR23" s="24"/>
     </row>
-    <row r="24" spans="1:154" ht="12" customHeight="1">
+    <row r="24" spans="1:156" ht="12" customHeight="1">
       <c r="DO24" s="35"/>
       <c r="DP24" s="24"/>
       <c r="DQ24" s="35"/>
       <c r="DR24" s="24"/>
     </row>
-    <row r="25" spans="1:154" ht="12" customHeight="1">
+    <row r="25" spans="1:156" ht="12" customHeight="1">
       <c r="DO25" s="35"/>
       <c r="DP25" s="24"/>
       <c r="DQ25" s="35"/>
       <c r="DR25" s="24"/>
     </row>
-    <row r="26" spans="1:154" ht="12" customHeight="1">
+    <row r="26" spans="1:156" ht="12" customHeight="1">
       <c r="DO26" s="35"/>
       <c r="DP26" s="24"/>
       <c r="DQ26" s="35"/>
@@ -9195,9 +9274,11 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:GC20"/>
+  <dimension ref="A1:GE20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="FV1" zoomScaleNormal="100" zoomScaleSheetLayoutView="85" workbookViewId="0">
+      <selection activeCell="GD10" sqref="GD10:GE20"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12" customHeight="1"/>
   <cols>
@@ -9278,7 +9359,7 @@
     <col min="183" max="16384" width="10.625" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="1" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A1" s="1" t="s">
         <v>155</v>
       </c>
@@ -9387,7 +9468,7 @@
       <c r="FX1" s="27"/>
       <c r="FZ1" s="27"/>
     </row>
-    <row r="2" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="2" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A2" s="1" t="s">
         <v>156</v>
       </c>
@@ -9496,7 +9577,7 @@
       <c r="FX2" s="27"/>
       <c r="FZ2" s="27"/>
     </row>
-    <row r="3" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="3" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A3" s="1" t="s">
         <v>157</v>
       </c>
@@ -9605,7 +9686,7 @@
       <c r="FX3" s="27"/>
       <c r="FZ3" s="27"/>
     </row>
-    <row r="4" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="4" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A4" s="1" t="s">
         <v>158</v>
       </c>
@@ -9714,7 +9795,7 @@
       <c r="FX4" s="27"/>
       <c r="FZ4" s="27"/>
     </row>
-    <row r="5" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="5" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="K5" s="27"/>
       <c r="L5" s="27"/>
       <c r="N5" s="27"/>
@@ -9788,7 +9869,7 @@
       <c r="FX5" s="27"/>
       <c r="FZ5" s="27"/>
     </row>
-    <row r="6" spans="1:185" s="2" customFormat="1" ht="12" customHeight="1">
+    <row r="6" spans="1:187" s="2" customFormat="1" ht="12" customHeight="1">
       <c r="A6"/>
       <c r="B6"/>
       <c r="C6"/>
@@ -9974,7 +10055,7 @@
       <c r="GB6"/>
       <c r="GC6"/>
     </row>
-    <row r="7" spans="1:185" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="7" spans="1:187" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="G7" s="2"/>
       <c r="H7" s="2"/>
       <c r="K7" s="32"/>
@@ -10055,7 +10136,7 @@
       <c r="FX7" s="32"/>
       <c r="FZ7" s="32"/>
     </row>
-    <row r="8" spans="1:185" s="43" customFormat="1">
+    <row r="8" spans="1:187" s="43" customFormat="1">
       <c r="B8" s="44"/>
       <c r="C8" s="44"/>
       <c r="D8" s="44"/>
@@ -10279,7 +10360,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="9" spans="1:185" s="43" customFormat="1">
+    <row r="9" spans="1:187" s="43" customFormat="1">
       <c r="A9" s="67"/>
       <c r="B9" s="55"/>
       <c r="C9" s="55"/>
@@ -10550,7 +10631,7 @@
       <c r="GB9" s="62"/>
       <c r="GC9" s="68"/>
     </row>
-    <row r="10" spans="1:185" s="43" customFormat="1">
+    <row r="10" spans="1:187" s="43" customFormat="1">
       <c r="A10" s="64" t="s">
         <v>0</v>
       </c>
@@ -11106,8 +11187,14 @@
       <c r="GC10" s="66" t="s">
         <v>119</v>
       </c>
+      <c r="GD10" s="65" t="s">
+        <v>188</v>
+      </c>
+      <c r="GE10" s="65" t="s">
+        <v>189</v>
+      </c>
     </row>
-    <row r="11" spans="1:185" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="11" spans="1:187" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -11292,8 +11379,10 @@
       <c r="GA11" s="4"/>
       <c r="GB11" s="4"/>
       <c r="GC11" s="4"/>
+      <c r="GD11" s="36"/>
+      <c r="GE11" s="36"/>
     </row>
-    <row r="12" spans="1:185" s="5" customFormat="1" ht="12" customHeight="1">
+    <row r="12" spans="1:187" s="5" customFormat="1" ht="12" customHeight="1">
       <c r="A12" s="9"/>
       <c r="B12" s="9"/>
       <c r="C12" s="9"/>
@@ -11478,8 +11567,10 @@
       <c r="GA12" s="9"/>
       <c r="GB12" s="9"/>
       <c r="GC12" s="9"/>
+      <c r="GD12" s="9"/>
+      <c r="GE12" s="9"/>
     </row>
-    <row r="13" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="13" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A13" s="10"/>
       <c r="B13" s="10"/>
       <c r="C13" s="10"/>
@@ -11665,8 +11756,10 @@
       <c r="GA13" s="10"/>
       <c r="GB13" s="10"/>
       <c r="GC13" s="10"/>
+      <c r="GD13" s="10"/>
+      <c r="GE13" s="10"/>
     </row>
-    <row r="14" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="14" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A14" s="10"/>
       <c r="B14" s="10"/>
       <c r="C14" s="10"/>
@@ -11852,8 +11945,10 @@
       <c r="GA14" s="10"/>
       <c r="GB14" s="10"/>
       <c r="GC14" s="10"/>
+      <c r="GD14" s="10"/>
+      <c r="GE14" s="10"/>
     </row>
-    <row r="15" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="15" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A15" s="10"/>
       <c r="B15" s="10"/>
       <c r="C15" s="10"/>
@@ -12039,8 +12134,10 @@
       <c r="GA15" s="10"/>
       <c r="GB15" s="10"/>
       <c r="GC15" s="10"/>
+      <c r="GD15" s="10"/>
+      <c r="GE15" s="10"/>
     </row>
-    <row r="16" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="16" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A16" s="10"/>
       <c r="B16" s="10"/>
       <c r="C16" s="10"/>
@@ -12226,8 +12323,10 @@
       <c r="GA16" s="10"/>
       <c r="GB16" s="10"/>
       <c r="GC16" s="10"/>
+      <c r="GD16" s="10"/>
+      <c r="GE16" s="10"/>
     </row>
-    <row r="17" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="17" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A17" s="10"/>
       <c r="B17" s="10"/>
       <c r="C17" s="10"/>
@@ -12421,8 +12520,10 @@
       <c r="GA17" s="10"/>
       <c r="GB17" s="10"/>
       <c r="GC17" s="10"/>
+      <c r="GD17" s="10"/>
+      <c r="GE17" s="10"/>
     </row>
-    <row r="18" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="18" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A18" s="10"/>
       <c r="B18" s="10"/>
       <c r="C18" s="10"/>
@@ -12624,8 +12725,10 @@
       <c r="GA18" s="10"/>
       <c r="GB18" s="10"/>
       <c r="GC18" s="10"/>
+      <c r="GD18" s="10"/>
+      <c r="GE18" s="10"/>
     </row>
-    <row r="19" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="19" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A19" s="10"/>
       <c r="B19" s="10"/>
       <c r="C19" s="10"/>
@@ -12811,8 +12914,10 @@
       <c r="GA19" s="10"/>
       <c r="GB19" s="10"/>
       <c r="GC19" s="10"/>
+      <c r="GD19" s="10"/>
+      <c r="GE19" s="10"/>
     </row>
-    <row r="20" spans="1:185" s="24" customFormat="1" ht="12" customHeight="1">
+    <row r="20" spans="1:187" s="24" customFormat="1" ht="12" customHeight="1">
       <c r="A20" s="13"/>
       <c r="B20" s="13"/>
       <c r="C20" s="13"/>
@@ -12998,6 +13103,8 @@
       <c r="GA20" s="13"/>
       <c r="GB20" s="13"/>
       <c r="GC20" s="13"/>
+      <c r="GD20" s="13"/>
+      <c r="GE20" s="13"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2"/>

</xml_diff>

<commit_message>
KMK003: MasterList: Fix bug #115504 + #115471
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="1260" windowWidth="16800" windowHeight="15375"/>
+    <workbookView xWindow="1605" yWindow="330" windowWidth="25605" windowHeight="15015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
     <sheet name="勤務形態 流動" sheetId="9" r:id="rId2"/>
     <sheet name="勤務形態 フレックス" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="187">
   <si>
     <t>コード</t>
   </si>
@@ -1086,16 +1095,6 @@
     <t>勤務形態 フレックス</t>
   </si>
   <si>
-    <t>半日勤務</t>
-    <rPh sb="0" eb="2">
-      <t>ハンニチ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンム</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>計算設定</t>
     <rPh sb="0" eb="2">
       <t>ケイサン</t>
@@ -1135,16 +1134,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>半日勤務</t>
-    <rPh sb="0" eb="2">
-      <t>ハンニチ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンム</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>　</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1168,6 +1157,19 @@
   </si>
   <si>
     <t>フレキシブルタイム</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>半日勤務を設定する</t>
+    <rPh sb="0" eb="2">
+      <t>ハンニチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キンム</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>セッテイ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1568,10 +1570,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1945,7 +1947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FM20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -3416,7 +3418,7 @@
       <c r="AB9" s="40"/>
       <c r="AC9" s="43"/>
       <c r="AD9" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="AE9" s="1" t="s">
         <v>31</v>
@@ -3490,11 +3492,11 @@
       <c r="BX9" s="38"/>
       <c r="BY9" s="39"/>
       <c r="BZ9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="CA9" s="39"/>
       <c r="CB9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CC9" s="27" t="s">
         <v>154</v>
@@ -3664,7 +3666,7 @@
         <v>16</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>14</v>
@@ -3849,13 +3851,13 @@
         <v>158</v>
       </c>
       <c r="BZ10" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="CA10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CB10" s="23" t="s">
         <v>181</v>
-      </c>
-      <c r="CA10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="CB10" s="23" t="s">
-        <v>183</v>
       </c>
       <c r="CC10" s="15" t="s">
         <v>26</v>
@@ -3917,12 +3919,8 @@
       <c r="CV10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="CW10" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="CX10" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="CW10" s="15"/>
+      <c r="CX10" s="15"/>
       <c r="CY10" s="15" t="s">
         <v>76</v>
       </c>
@@ -4199,7 +4197,7 @@
       <c r="BW11" s="13"/>
       <c r="BX11" s="31"/>
       <c r="BY11" s="13"/>
-      <c r="BZ11" s="57"/>
+      <c r="BZ11" s="58"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="55"/>
       <c r="CC11" s="35"/>
@@ -7187,7 +7185,7 @@
       <c r="AZ9" s="38"/>
       <c r="BA9" s="39"/>
       <c r="BB9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BC9" s="39"/>
       <c r="BD9" s="28"/>
@@ -7359,7 +7357,7 @@
         <v>15</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>14</v>
@@ -7475,10 +7473,10 @@
         <v>61</v>
       </c>
       <c r="BB10" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BC10" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BD10" s="47" t="s">
         <v>143</v>
@@ -7814,7 +7812,7 @@
       <c r="AY11" s="13"/>
       <c r="AZ11" s="31"/>
       <c r="BA11" s="13"/>
-      <c r="BB11" s="57"/>
+      <c r="BB11" s="58"/>
       <c r="BC11" s="55"/>
       <c r="BD11" s="13"/>
       <c r="BE11" s="35"/>
@@ -7887,8 +7885,8 @@
       <c r="DT11" s="13"/>
       <c r="DU11" s="13"/>
       <c r="DV11" s="13"/>
-      <c r="DW11" s="57"/>
-      <c r="DX11" s="57"/>
+      <c r="DW11" s="58"/>
+      <c r="DX11" s="58"/>
       <c r="DY11" s="31"/>
       <c r="DZ11" s="13"/>
       <c r="EA11" s="13"/>
@@ -9323,7 +9321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FW20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -10645,7 +10643,7 @@
       <c r="Y8" s="38"/>
       <c r="Z8" s="39"/>
       <c r="AA8" s="56" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AB8" s="37"/>
       <c r="AC8" s="38"/>
@@ -10875,7 +10873,7 @@
       <c r="Y9" s="38"/>
       <c r="Z9" s="39"/>
       <c r="AA9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="AB9" s="27" t="s">
         <v>154</v>
@@ -10896,7 +10894,7 @@
       <c r="AL9" s="40"/>
       <c r="AM9" s="43"/>
       <c r="AN9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="AO9" s="25" t="s">
         <v>154</v>
@@ -10953,11 +10951,11 @@
       <c r="BW9" s="38"/>
       <c r="BX9" s="39"/>
       <c r="BY9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BZ9" s="39"/>
       <c r="CA9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CB9" s="14" t="s">
         <v>143</v>
@@ -11153,10 +11151,10 @@
         <v>15</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>152</v>
@@ -11332,15 +11330,15 @@
         <v>61</v>
       </c>
       <c r="BY10" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="BZ10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CA10" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="BZ10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="CA10" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="CB10" s="58"/>
+      <c r="CB10" s="57"/>
       <c r="CC10" s="15" t="s">
         <v>26</v>
       </c>
@@ -11653,10 +11651,10 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
@@ -11666,7 +11664,7 @@
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
-      <c r="AA11" s="57"/>
+      <c r="AA11" s="58"/>
       <c r="AB11" s="34"/>
       <c r="AC11" s="35"/>
       <c r="AD11" s="35"/>
@@ -11679,7 +11677,7 @@
       <c r="AK11" s="35"/>
       <c r="AL11" s="35"/>
       <c r="AM11" s="15"/>
-      <c r="AN11" s="57"/>
+      <c r="AN11" s="58"/>
       <c r="AO11" s="35"/>
       <c r="AP11" s="35"/>
       <c r="AQ11" s="35"/>
@@ -11716,7 +11714,7 @@
       <c r="BV11" s="13"/>
       <c r="BW11" s="31"/>
       <c r="BX11" s="13"/>
-      <c r="BY11" s="57"/>
+      <c r="BY11" s="58"/>
       <c r="BZ11" s="55"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="13"/>
@@ -11791,9 +11789,9 @@
       <c r="ES11" s="13"/>
       <c r="ET11" s="31"/>
       <c r="EU11" s="13"/>
-      <c r="EV11" s="57"/>
+      <c r="EV11" s="58"/>
       <c r="EW11" s="13"/>
-      <c r="EX11" s="57"/>
+      <c r="EX11" s="58"/>
       <c r="EY11" s="13"/>
       <c r="EZ11" s="13"/>
       <c r="FA11" s="13"/>

</xml_diff>

<commit_message>
Revert "KMK003: MasterList: Fix bug #115504 + #115471"
This reverts commit 8d97a66a20c78217f3976125411a16386d5ae188.
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -1,36 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="330" windowWidth="25605" windowHeight="15015" activeTab="2"/>
+    <workbookView xWindow="3765" yWindow="1260" windowWidth="16800" windowHeight="15375"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
     <sheet name="勤務形態 流動" sheetId="9" r:id="rId2"/>
     <sheet name="勤務形態 フレックス" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="188">
   <si>
     <t>コード</t>
   </si>
@@ -1095,6 +1086,16 @@
     <t>勤務形態 フレックス</t>
   </si>
   <si>
+    <t>半日勤務</t>
+    <rPh sb="0" eb="2">
+      <t>ハンニチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キンム</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>計算設定</t>
     <rPh sb="0" eb="2">
       <t>ケイサン</t>
@@ -1134,6 +1135,16 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
+    <t>半日勤務</t>
+    <rPh sb="0" eb="2">
+      <t>ハンニチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キンム</t>
+    </rPh>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
     <t>　</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1157,19 +1168,6 @@
   </si>
   <si>
     <t>フレキシブルタイム</t>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
-    <t>半日勤務を設定する</t>
-    <rPh sb="0" eb="2">
-      <t>ハンニチ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンム</t>
-    </rPh>
-    <rPh sb="5" eb="7">
-      <t>セッテイ</t>
-    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1570,10 +1568,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1947,7 +1945,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FM20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -3418,7 +3416,7 @@
       <c r="AB9" s="40"/>
       <c r="AC9" s="43"/>
       <c r="AD9" s="1" t="s">
-        <v>186</v>
+        <v>178</v>
       </c>
       <c r="AE9" s="1" t="s">
         <v>31</v>
@@ -3492,11 +3490,11 @@
       <c r="BX9" s="38"/>
       <c r="BY9" s="39"/>
       <c r="BZ9" s="38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="CA9" s="39"/>
       <c r="CB9" s="56" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="CC9" s="27" t="s">
         <v>154</v>
@@ -3666,7 +3664,7 @@
         <v>16</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>14</v>
@@ -3851,13 +3849,13 @@
         <v>158</v>
       </c>
       <c r="BZ10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="CA10" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="CA10" s="15" t="s">
-        <v>179</v>
-      </c>
       <c r="CB10" s="23" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
       <c r="CC10" s="15" t="s">
         <v>26</v>
@@ -3919,8 +3917,12 @@
       <c r="CV10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="CW10" s="15"/>
-      <c r="CX10" s="15"/>
+      <c r="CW10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CX10" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="CY10" s="15" t="s">
         <v>76</v>
       </c>
@@ -4197,7 +4199,7 @@
       <c r="BW11" s="13"/>
       <c r="BX11" s="31"/>
       <c r="BY11" s="13"/>
-      <c r="BZ11" s="58"/>
+      <c r="BZ11" s="57"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="55"/>
       <c r="CC11" s="35"/>
@@ -7185,7 +7187,7 @@
       <c r="AZ9" s="38"/>
       <c r="BA9" s="39"/>
       <c r="BB9" s="38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="BC9" s="39"/>
       <c r="BD9" s="28"/>
@@ -7357,7 +7359,7 @@
         <v>15</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>14</v>
@@ -7473,10 +7475,10 @@
         <v>61</v>
       </c>
       <c r="BB10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="BC10" s="15" t="s">
         <v>180</v>
-      </c>
-      <c r="BC10" s="15" t="s">
-        <v>179</v>
       </c>
       <c r="BD10" s="47" t="s">
         <v>143</v>
@@ -7812,7 +7814,7 @@
       <c r="AY11" s="13"/>
       <c r="AZ11" s="31"/>
       <c r="BA11" s="13"/>
-      <c r="BB11" s="58"/>
+      <c r="BB11" s="57"/>
       <c r="BC11" s="55"/>
       <c r="BD11" s="13"/>
       <c r="BE11" s="35"/>
@@ -7885,8 +7887,8 @@
       <c r="DT11" s="13"/>
       <c r="DU11" s="13"/>
       <c r="DV11" s="13"/>
-      <c r="DW11" s="58"/>
-      <c r="DX11" s="58"/>
+      <c r="DW11" s="57"/>
+      <c r="DX11" s="57"/>
       <c r="DY11" s="31"/>
       <c r="DZ11" s="13"/>
       <c r="EA11" s="13"/>
@@ -9321,7 +9323,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FW20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -10643,7 +10645,7 @@
       <c r="Y8" s="38"/>
       <c r="Z8" s="39"/>
       <c r="AA8" s="56" t="s">
-        <v>185</v>
+        <v>187</v>
       </c>
       <c r="AB8" s="37"/>
       <c r="AC8" s="38"/>
@@ -10873,7 +10875,7 @@
       <c r="Y9" s="38"/>
       <c r="Z9" s="39"/>
       <c r="AA9" s="56" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AB9" s="27" t="s">
         <v>154</v>
@@ -10894,7 +10896,7 @@
       <c r="AL9" s="40"/>
       <c r="AM9" s="43"/>
       <c r="AN9" s="56" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="AO9" s="25" t="s">
         <v>154</v>
@@ -10951,11 +10953,11 @@
       <c r="BW9" s="38"/>
       <c r="BX9" s="39"/>
       <c r="BY9" s="38" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="BZ9" s="39"/>
       <c r="CA9" s="56" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="CB9" s="14" t="s">
         <v>143</v>
@@ -11151,10 +11153,10 @@
         <v>15</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>183</v>
+        <v>185</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>184</v>
+        <v>186</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>152</v>
@@ -11330,15 +11332,15 @@
         <v>61</v>
       </c>
       <c r="BY10" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="BZ10" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="BZ10" s="15" t="s">
-        <v>179</v>
-      </c>
       <c r="CA10" s="23" t="s">
-        <v>181</v>
-      </c>
-      <c r="CB10" s="57"/>
+        <v>183</v>
+      </c>
+      <c r="CB10" s="58"/>
       <c r="CC10" s="15" t="s">
         <v>26</v>
       </c>
@@ -11651,10 +11653,10 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
-      <c r="P11" s="58"/>
-      <c r="Q11" s="58"/>
+      <c r="N11" s="57"/>
+      <c r="O11" s="57"/>
+      <c r="P11" s="57"/>
+      <c r="Q11" s="57"/>
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
@@ -11664,7 +11666,7 @@
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
-      <c r="AA11" s="58"/>
+      <c r="AA11" s="57"/>
       <c r="AB11" s="34"/>
       <c r="AC11" s="35"/>
       <c r="AD11" s="35"/>
@@ -11677,7 +11679,7 @@
       <c r="AK11" s="35"/>
       <c r="AL11" s="35"/>
       <c r="AM11" s="15"/>
-      <c r="AN11" s="58"/>
+      <c r="AN11" s="57"/>
       <c r="AO11" s="35"/>
       <c r="AP11" s="35"/>
       <c r="AQ11" s="35"/>
@@ -11714,7 +11716,7 @@
       <c r="BV11" s="13"/>
       <c r="BW11" s="31"/>
       <c r="BX11" s="13"/>
-      <c r="BY11" s="58"/>
+      <c r="BY11" s="57"/>
       <c r="BZ11" s="55"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="13"/>
@@ -11789,9 +11791,9 @@
       <c r="ES11" s="13"/>
       <c r="ET11" s="31"/>
       <c r="EU11" s="13"/>
-      <c r="EV11" s="58"/>
+      <c r="EV11" s="57"/>
       <c r="EW11" s="13"/>
-      <c r="EX11" s="58"/>
+      <c r="EX11" s="57"/>
       <c r="EY11" s="13"/>
       <c r="EZ11" s="13"/>
       <c r="FA11" s="13"/>

</xml_diff>

<commit_message>
KMK003: MasterList: Change position template
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -1,27 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="3765" yWindow="1260" windowWidth="16800" windowHeight="15375"/>
+    <workbookView xWindow="1605" yWindow="330" windowWidth="25605" windowHeight="15015" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
     <sheet name="勤務形態 流動" sheetId="9" r:id="rId2"/>
     <sheet name="勤務形態 フレックス" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="187">
   <si>
     <t>コード</t>
   </si>
@@ -1086,16 +1095,6 @@
     <t>勤務形態 フレックス</t>
   </si>
   <si>
-    <t>半日勤務</t>
-    <rPh sb="0" eb="2">
-      <t>ハンニチ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンム</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>計算設定</t>
     <rPh sb="0" eb="2">
       <t>ケイサン</t>
@@ -1135,16 +1134,6 @@
     <phoneticPr fontId="2"/>
   </si>
   <si>
-    <t>半日勤務</t>
-    <rPh sb="0" eb="2">
-      <t>ハンニチ</t>
-    </rPh>
-    <rPh sb="2" eb="4">
-      <t>キンム</t>
-    </rPh>
-    <phoneticPr fontId="2"/>
-  </si>
-  <si>
     <t>　</t>
     <phoneticPr fontId="2"/>
   </si>
@@ -1168,6 +1157,19 @@
   </si>
   <si>
     <t>フレキシブルタイム</t>
+    <phoneticPr fontId="2"/>
+  </si>
+  <si>
+    <t>半日勤務を設定する</t>
+    <rPh sb="0" eb="2">
+      <t>ハンニチ</t>
+    </rPh>
+    <rPh sb="2" eb="4">
+      <t>キンム</t>
+    </rPh>
+    <rPh sb="5" eb="7">
+      <t>セッテイ</t>
+    </rPh>
     <phoneticPr fontId="2"/>
   </si>
 </sst>
@@ -1568,10 +1570,10 @@
     <xf numFmtId="49" fontId="3" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1945,7 +1947,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FM20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -3416,7 +3418,7 @@
       <c r="AB9" s="40"/>
       <c r="AC9" s="43"/>
       <c r="AD9" s="1" t="s">
-        <v>178</v>
+        <v>186</v>
       </c>
       <c r="AE9" s="1" t="s">
         <v>31</v>
@@ -3490,11 +3492,11 @@
       <c r="BX9" s="38"/>
       <c r="BY9" s="39"/>
       <c r="BZ9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="CA9" s="39"/>
       <c r="CB9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CC9" s="27" t="s">
         <v>154</v>
@@ -3664,7 +3666,7 @@
         <v>16</v>
       </c>
       <c r="O10" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="P10" s="15" t="s">
         <v>14</v>
@@ -3849,13 +3851,13 @@
         <v>158</v>
       </c>
       <c r="BZ10" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="CA10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CB10" s="23" t="s">
         <v>181</v>
-      </c>
-      <c r="CA10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="CB10" s="23" t="s">
-        <v>183</v>
       </c>
       <c r="CC10" s="15" t="s">
         <v>26</v>
@@ -3917,12 +3919,8 @@
       <c r="CV10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="CW10" s="15" t="s">
-        <v>77</v>
-      </c>
-      <c r="CX10" s="15" t="s">
-        <v>79</v>
-      </c>
+      <c r="CW10" s="15"/>
+      <c r="CX10" s="15"/>
       <c r="CY10" s="15" t="s">
         <v>76</v>
       </c>
@@ -4199,7 +4197,7 @@
       <c r="BW11" s="13"/>
       <c r="BX11" s="31"/>
       <c r="BY11" s="13"/>
-      <c r="BZ11" s="57"/>
+      <c r="BZ11" s="58"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="55"/>
       <c r="CC11" s="35"/>
@@ -7187,7 +7185,7 @@
       <c r="AZ9" s="38"/>
       <c r="BA9" s="39"/>
       <c r="BB9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BC9" s="39"/>
       <c r="BD9" s="28"/>
@@ -7359,7 +7357,7 @@
         <v>15</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="O10" s="15" t="s">
         <v>14</v>
@@ -7475,10 +7473,10 @@
         <v>61</v>
       </c>
       <c r="BB10" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="BC10" s="15" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="BD10" s="47" t="s">
         <v>143</v>
@@ -7814,7 +7812,7 @@
       <c r="AY11" s="13"/>
       <c r="AZ11" s="31"/>
       <c r="BA11" s="13"/>
-      <c r="BB11" s="57"/>
+      <c r="BB11" s="58"/>
       <c r="BC11" s="55"/>
       <c r="BD11" s="13"/>
       <c r="BE11" s="35"/>
@@ -7887,8 +7885,8 @@
       <c r="DT11" s="13"/>
       <c r="DU11" s="13"/>
       <c r="DV11" s="13"/>
-      <c r="DW11" s="57"/>
-      <c r="DX11" s="57"/>
+      <c r="DW11" s="58"/>
+      <c r="DX11" s="58"/>
       <c r="DY11" s="31"/>
       <c r="DZ11" s="13"/>
       <c r="EA11" s="13"/>
@@ -9323,7 +9321,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FW20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.625" defaultRowHeight="12"/>
   <cols>
@@ -10645,7 +10643,7 @@
       <c r="Y8" s="38"/>
       <c r="Z8" s="39"/>
       <c r="AA8" s="56" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="AB8" s="37"/>
       <c r="AC8" s="38"/>
@@ -10875,7 +10873,7 @@
       <c r="Y9" s="38"/>
       <c r="Z9" s="39"/>
       <c r="AA9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="AB9" s="27" t="s">
         <v>154</v>
@@ -10896,7 +10894,7 @@
       <c r="AL9" s="40"/>
       <c r="AM9" s="43"/>
       <c r="AN9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="AO9" s="25" t="s">
         <v>154</v>
@@ -10953,11 +10951,11 @@
       <c r="BW9" s="38"/>
       <c r="BX9" s="39"/>
       <c r="BY9" s="38" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="BZ9" s="39"/>
       <c r="CA9" s="56" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="CB9" s="14" t="s">
         <v>143</v>
@@ -11153,10 +11151,10 @@
         <v>15</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="Q10" s="15" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="R10" s="15" t="s">
         <v>152</v>
@@ -11332,15 +11330,15 @@
         <v>61</v>
       </c>
       <c r="BY10" s="15" t="s">
+        <v>180</v>
+      </c>
+      <c r="BZ10" s="15" t="s">
+        <v>179</v>
+      </c>
+      <c r="CA10" s="23" t="s">
         <v>181</v>
       </c>
-      <c r="BZ10" s="15" t="s">
-        <v>180</v>
-      </c>
-      <c r="CA10" s="23" t="s">
-        <v>183</v>
-      </c>
-      <c r="CB10" s="58"/>
+      <c r="CB10" s="57"/>
       <c r="CC10" s="15" t="s">
         <v>26</v>
       </c>
@@ -11653,10 +11651,10 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="57"/>
-      <c r="O11" s="57"/>
-      <c r="P11" s="57"/>
-      <c r="Q11" s="57"/>
+      <c r="N11" s="58"/>
+      <c r="O11" s="58"/>
+      <c r="P11" s="58"/>
+      <c r="Q11" s="58"/>
       <c r="R11" s="31"/>
       <c r="S11" s="31"/>
       <c r="T11" s="31"/>
@@ -11666,7 +11664,7 @@
       <c r="X11" s="31"/>
       <c r="Y11" s="31"/>
       <c r="Z11" s="31"/>
-      <c r="AA11" s="57"/>
+      <c r="AA11" s="58"/>
       <c r="AB11" s="34"/>
       <c r="AC11" s="35"/>
       <c r="AD11" s="35"/>
@@ -11679,7 +11677,7 @@
       <c r="AK11" s="35"/>
       <c r="AL11" s="35"/>
       <c r="AM11" s="15"/>
-      <c r="AN11" s="57"/>
+      <c r="AN11" s="58"/>
       <c r="AO11" s="35"/>
       <c r="AP11" s="35"/>
       <c r="AQ11" s="35"/>
@@ -11716,7 +11714,7 @@
       <c r="BV11" s="13"/>
       <c r="BW11" s="31"/>
       <c r="BX11" s="13"/>
-      <c r="BY11" s="57"/>
+      <c r="BY11" s="58"/>
       <c r="BZ11" s="55"/>
       <c r="CA11" s="55"/>
       <c r="CB11" s="13"/>
@@ -11791,9 +11789,9 @@
       <c r="ES11" s="13"/>
       <c r="ET11" s="31"/>
       <c r="EU11" s="13"/>
-      <c r="EV11" s="57"/>
+      <c r="EV11" s="58"/>
       <c r="EW11" s="13"/>
-      <c r="EX11" s="57"/>
+      <c r="EX11" s="58"/>
       <c r="EY11" s="13"/>
       <c r="EZ11" s="13"/>
       <c r="FA11" s="13"/>

</xml_diff>

<commit_message>
KMK003: MasterList: Update template #115514
</commit_message>
<xml_diff>
--- a/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
+++ b/nts.uk/uk.at/at.file/nts.uk.file.at.infra/src/main/resources/report/KMK003.xlsx
@@ -4,14 +4,14 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="1605" yWindow="330" windowWidth="25605" windowHeight="15015" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11685" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="勤務形態 通常" sheetId="1" r:id="rId1"/>
     <sheet name="勤務形態 流動" sheetId="9" r:id="rId2"/>
     <sheet name="勤務形態 フレックス" sheetId="11" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="695" uniqueCount="187">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="697" uniqueCount="187">
   <si>
     <t>コード</t>
   </si>
@@ -3919,8 +3919,12 @@
       <c r="CV10" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="CW10" s="15"/>
-      <c r="CX10" s="15"/>
+      <c r="CW10" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="CX10" s="15" t="s">
+        <v>79</v>
+      </c>
       <c r="CY10" s="15" t="s">
         <v>76</v>
       </c>
@@ -7836,8 +7840,8 @@
       <c r="BW11" s="35"/>
       <c r="BX11" s="15"/>
       <c r="BY11" s="13"/>
-      <c r="BZ11" s="15"/>
-      <c r="CA11" s="15"/>
+      <c r="BZ11" s="35"/>
+      <c r="CA11" s="35"/>
       <c r="CB11" s="35"/>
       <c r="CC11" s="35"/>
       <c r="CD11" s="13"/>
@@ -7885,8 +7889,8 @@
       <c r="DT11" s="13"/>
       <c r="DU11" s="13"/>
       <c r="DV11" s="13"/>
-      <c r="DW11" s="58"/>
-      <c r="DX11" s="58"/>
+      <c r="DW11" s="31"/>
+      <c r="DX11" s="31"/>
       <c r="DY11" s="31"/>
       <c r="DZ11" s="13"/>
       <c r="EA11" s="13"/>
@@ -7986,8 +7990,8 @@
       <c r="BW12" s="35"/>
       <c r="BX12" s="15"/>
       <c r="BY12" s="22"/>
-      <c r="BZ12" s="15"/>
-      <c r="CA12" s="15"/>
+      <c r="BZ12" s="35"/>
+      <c r="CA12" s="35"/>
       <c r="CB12" s="35"/>
       <c r="CC12" s="35"/>
       <c r="CD12" s="22"/>
@@ -8035,8 +8039,8 @@
       <c r="DT12" s="22"/>
       <c r="DU12" s="22"/>
       <c r="DV12" s="22"/>
-      <c r="DW12" s="22"/>
-      <c r="DX12" s="22"/>
+      <c r="DW12" s="49"/>
+      <c r="DX12" s="49"/>
       <c r="DY12" s="49"/>
       <c r="DZ12" s="22"/>
       <c r="EA12" s="22"/>
@@ -8136,8 +8140,8 @@
       <c r="BW13" s="35"/>
       <c r="BX13" s="15"/>
       <c r="BY13" s="22"/>
-      <c r="BZ13" s="15"/>
-      <c r="CA13" s="15"/>
+      <c r="BZ13" s="35"/>
+      <c r="CA13" s="35"/>
       <c r="CB13" s="35"/>
       <c r="CC13" s="35"/>
       <c r="CD13" s="22"/>
@@ -8185,8 +8189,8 @@
       <c r="DT13" s="22"/>
       <c r="DU13" s="22"/>
       <c r="DV13" s="22"/>
-      <c r="DW13" s="22"/>
-      <c r="DX13" s="22"/>
+      <c r="DW13" s="49"/>
+      <c r="DX13" s="49"/>
       <c r="DY13" s="49"/>
       <c r="DZ13" s="22"/>
       <c r="EA13" s="22"/>
@@ -8286,8 +8290,8 @@
       <c r="BW14" s="35"/>
       <c r="BX14" s="15"/>
       <c r="BY14" s="22"/>
-      <c r="BZ14" s="15"/>
-      <c r="CA14" s="15"/>
+      <c r="BZ14" s="35"/>
+      <c r="CA14" s="35"/>
       <c r="CB14" s="35"/>
       <c r="CC14" s="35"/>
       <c r="CD14" s="16"/>
@@ -8335,8 +8339,8 @@
       <c r="DT14" s="16"/>
       <c r="DU14" s="16"/>
       <c r="DV14" s="16"/>
-      <c r="DW14" s="16"/>
-      <c r="DX14" s="16"/>
+      <c r="DW14" s="32"/>
+      <c r="DX14" s="32"/>
       <c r="DY14" s="32"/>
       <c r="DZ14" s="16"/>
       <c r="EA14" s="16"/>
@@ -8436,8 +8440,8 @@
       <c r="BW15" s="35"/>
       <c r="BX15" s="15"/>
       <c r="BY15" s="22"/>
-      <c r="BZ15" s="15"/>
-      <c r="CA15" s="15"/>
+      <c r="BZ15" s="35"/>
+      <c r="CA15" s="35"/>
       <c r="CB15" s="35"/>
       <c r="CC15" s="35"/>
       <c r="CD15" s="16"/>
@@ -8485,8 +8489,8 @@
       <c r="DT15" s="16"/>
       <c r="DU15" s="16"/>
       <c r="DV15" s="16"/>
-      <c r="DW15" s="16"/>
-      <c r="DX15" s="16"/>
+      <c r="DW15" s="32"/>
+      <c r="DX15" s="32"/>
       <c r="DY15" s="32"/>
       <c r="DZ15" s="16"/>
       <c r="EA15" s="16"/>
@@ -8586,8 +8590,8 @@
       <c r="BW16" s="35"/>
       <c r="BX16" s="15"/>
       <c r="BY16" s="22"/>
-      <c r="BZ16" s="15"/>
-      <c r="CA16" s="15"/>
+      <c r="BZ16" s="35"/>
+      <c r="CA16" s="35"/>
       <c r="CB16" s="22"/>
       <c r="CC16" s="22"/>
       <c r="CD16" s="16"/>
@@ -8635,8 +8639,8 @@
       <c r="DT16" s="16"/>
       <c r="DU16" s="16"/>
       <c r="DV16" s="16"/>
-      <c r="DW16" s="16"/>
-      <c r="DX16" s="16"/>
+      <c r="DW16" s="32"/>
+      <c r="DX16" s="32"/>
       <c r="DY16" s="32"/>
       <c r="DZ16" s="16"/>
       <c r="EA16" s="16"/>
@@ -8738,8 +8742,8 @@
       <c r="BW17" s="35"/>
       <c r="BX17" s="15"/>
       <c r="BY17" s="22"/>
-      <c r="BZ17" s="15"/>
-      <c r="CA17" s="15"/>
+      <c r="BZ17" s="35"/>
+      <c r="CA17" s="35"/>
       <c r="CB17" s="11" t="s">
         <v>150</v>
       </c>
@@ -8789,8 +8793,8 @@
       <c r="DT17" s="16"/>
       <c r="DU17" s="16"/>
       <c r="DV17" s="16"/>
-      <c r="DW17" s="16"/>
-      <c r="DX17" s="16"/>
+      <c r="DW17" s="32"/>
+      <c r="DX17" s="32"/>
       <c r="DY17" s="32"/>
       <c r="DZ17" s="16"/>
       <c r="EA17" s="16"/>
@@ -8894,8 +8898,8 @@
       <c r="BW18" s="35"/>
       <c r="BX18" s="15"/>
       <c r="BY18" s="22"/>
-      <c r="BZ18" s="15"/>
-      <c r="CA18" s="15"/>
+      <c r="BZ18" s="35"/>
+      <c r="CA18" s="35"/>
       <c r="CB18" s="12" t="s">
         <v>140</v>
       </c>
@@ -8947,8 +8951,8 @@
       <c r="DT18" s="16"/>
       <c r="DU18" s="16"/>
       <c r="DV18" s="16"/>
-      <c r="DW18" s="16"/>
-      <c r="DX18" s="16"/>
+      <c r="DW18" s="32"/>
+      <c r="DX18" s="32"/>
       <c r="DY18" s="32"/>
       <c r="DZ18" s="16"/>
       <c r="EA18" s="16"/>
@@ -9048,8 +9052,8 @@
       <c r="BW19" s="35"/>
       <c r="BX19" s="15"/>
       <c r="BY19" s="22"/>
-      <c r="BZ19" s="15"/>
-      <c r="CA19" s="15"/>
+      <c r="BZ19" s="35"/>
+      <c r="CA19" s="35"/>
       <c r="CB19" s="35"/>
       <c r="CC19" s="35"/>
       <c r="CD19" s="16"/>
@@ -9097,8 +9101,8 @@
       <c r="DT19" s="16"/>
       <c r="DU19" s="16"/>
       <c r="DV19" s="16"/>
-      <c r="DW19" s="16"/>
-      <c r="DX19" s="16"/>
+      <c r="DW19" s="32"/>
+      <c r="DX19" s="32"/>
       <c r="DY19" s="32"/>
       <c r="DZ19" s="16"/>
       <c r="EA19" s="16"/>
@@ -9198,8 +9202,8 @@
       <c r="BW20" s="35"/>
       <c r="BX20" s="15"/>
       <c r="BY20" s="23"/>
-      <c r="BZ20" s="15"/>
-      <c r="CA20" s="15"/>
+      <c r="BZ20" s="35"/>
+      <c r="CA20" s="35"/>
       <c r="CB20" s="23"/>
       <c r="CC20" s="23"/>
       <c r="CD20" s="18"/>
@@ -9247,8 +9251,8 @@
       <c r="DT20" s="18"/>
       <c r="DU20" s="18"/>
       <c r="DV20" s="18"/>
-      <c r="DW20" s="18"/>
-      <c r="DX20" s="18"/>
+      <c r="DW20" s="33"/>
+      <c r="DX20" s="33"/>
       <c r="DY20" s="33"/>
       <c r="DZ20" s="18"/>
       <c r="EA20" s="18"/>
@@ -11651,8 +11655,8 @@
       <c r="K11" s="31"/>
       <c r="L11" s="31"/>
       <c r="M11" s="13"/>
-      <c r="N11" s="58"/>
-      <c r="O11" s="58"/>
+      <c r="N11" s="31"/>
+      <c r="O11" s="31"/>
       <c r="P11" s="58"/>
       <c r="Q11" s="58"/>
       <c r="R11" s="31"/>
@@ -11789,7 +11793,7 @@
       <c r="ES11" s="13"/>
       <c r="ET11" s="31"/>
       <c r="EU11" s="13"/>
-      <c r="EV11" s="58"/>
+      <c r="EV11" s="31"/>
       <c r="EW11" s="13"/>
       <c r="EX11" s="58"/>
       <c r="EY11" s="13"/>
@@ -11832,8 +11836,8 @@
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
       <c r="M12" s="22"/>
-      <c r="N12" s="22"/>
-      <c r="O12" s="22"/>
+      <c r="N12" s="49"/>
+      <c r="O12" s="49"/>
       <c r="P12" s="22"/>
       <c r="Q12" s="22"/>
       <c r="R12" s="49"/>
@@ -11970,7 +11974,7 @@
       <c r="ES12" s="22"/>
       <c r="ET12" s="49"/>
       <c r="EU12" s="22"/>
-      <c r="EV12" s="22"/>
+      <c r="EV12" s="49"/>
       <c r="EW12" s="22"/>
       <c r="EX12" s="22"/>
       <c r="EY12" s="22"/>
@@ -12013,8 +12017,8 @@
       <c r="K13" s="32"/>
       <c r="L13" s="32"/>
       <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
+      <c r="N13" s="32"/>
+      <c r="O13" s="32"/>
       <c r="P13" s="16"/>
       <c r="Q13" s="16"/>
       <c r="R13" s="32"/>
@@ -12151,7 +12155,7 @@
       <c r="ES13" s="16"/>
       <c r="ET13" s="32"/>
       <c r="EU13" s="16"/>
-      <c r="EV13" s="16"/>
+      <c r="EV13" s="32"/>
       <c r="EW13" s="16"/>
       <c r="EX13" s="16"/>
       <c r="EY13" s="16"/>
@@ -12194,8 +12198,8 @@
       <c r="K14" s="32"/>
       <c r="L14" s="32"/>
       <c r="M14" s="16"/>
-      <c r="N14" s="16"/>
-      <c r="O14" s="16"/>
+      <c r="N14" s="32"/>
+      <c r="O14" s="32"/>
       <c r="P14" s="16"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="32"/>
@@ -12332,7 +12336,7 @@
       <c r="ES14" s="16"/>
       <c r="ET14" s="32"/>
       <c r="EU14" s="16"/>
-      <c r="EV14" s="16"/>
+      <c r="EV14" s="32"/>
       <c r="EW14" s="16"/>
       <c r="EX14" s="16"/>
       <c r="EY14" s="16"/>
@@ -12375,8 +12379,8 @@
       <c r="K15" s="32"/>
       <c r="L15" s="32"/>
       <c r="M15" s="16"/>
-      <c r="N15" s="16"/>
-      <c r="O15" s="16"/>
+      <c r="N15" s="32"/>
+      <c r="O15" s="32"/>
       <c r="P15" s="16"/>
       <c r="Q15" s="16"/>
       <c r="R15" s="32"/>
@@ -12513,7 +12517,7 @@
       <c r="ES15" s="16"/>
       <c r="ET15" s="32"/>
       <c r="EU15" s="16"/>
-      <c r="EV15" s="16"/>
+      <c r="EV15" s="32"/>
       <c r="EW15" s="16"/>
       <c r="EX15" s="16"/>
       <c r="EY15" s="16"/>
@@ -12556,8 +12560,8 @@
       <c r="K16" s="32"/>
       <c r="L16" s="32"/>
       <c r="M16" s="16"/>
-      <c r="N16" s="16"/>
-      <c r="O16" s="16"/>
+      <c r="N16" s="32"/>
+      <c r="O16" s="32"/>
       <c r="P16" s="16"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="32"/>
@@ -12694,7 +12698,7 @@
       <c r="ES16" s="16"/>
       <c r="ET16" s="32"/>
       <c r="EU16" s="16"/>
-      <c r="EV16" s="16"/>
+      <c r="EV16" s="32"/>
       <c r="EW16" s="16"/>
       <c r="EX16" s="16"/>
       <c r="EY16" s="16"/>
@@ -12737,8 +12741,8 @@
       <c r="K17" s="32"/>
       <c r="L17" s="32"/>
       <c r="M17" s="16"/>
-      <c r="N17" s="16"/>
-      <c r="O17" s="16"/>
+      <c r="N17" s="32"/>
+      <c r="O17" s="32"/>
       <c r="P17" s="16"/>
       <c r="Q17" s="16"/>
       <c r="R17" s="32"/>
@@ -12883,7 +12887,7 @@
       <c r="ES17" s="16"/>
       <c r="ET17" s="32"/>
       <c r="EU17" s="16"/>
-      <c r="EV17" s="16"/>
+      <c r="EV17" s="32"/>
       <c r="EW17" s="16"/>
       <c r="EX17" s="16"/>
       <c r="EY17" s="16"/>
@@ -12926,8 +12930,8 @@
       <c r="K18" s="32"/>
       <c r="L18" s="32"/>
       <c r="M18" s="16"/>
-      <c r="N18" s="16"/>
-      <c r="O18" s="16"/>
+      <c r="N18" s="32"/>
+      <c r="O18" s="32"/>
       <c r="P18" s="16"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="32"/>
@@ -13080,7 +13084,7 @@
       <c r="ES18" s="16"/>
       <c r="ET18" s="32"/>
       <c r="EU18" s="16"/>
-      <c r="EV18" s="16"/>
+      <c r="EV18" s="32"/>
       <c r="EW18" s="16"/>
       <c r="EX18" s="16"/>
       <c r="EY18" s="16"/>
@@ -13123,8 +13127,8 @@
       <c r="K19" s="32"/>
       <c r="L19" s="32"/>
       <c r="M19" s="16"/>
-      <c r="N19" s="16"/>
-      <c r="O19" s="16"/>
+      <c r="N19" s="32"/>
+      <c r="O19" s="32"/>
       <c r="P19" s="16"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="32"/>
@@ -13261,7 +13265,7 @@
       <c r="ES19" s="16"/>
       <c r="ET19" s="32"/>
       <c r="EU19" s="16"/>
-      <c r="EV19" s="16"/>
+      <c r="EV19" s="32"/>
       <c r="EW19" s="16"/>
       <c r="EX19" s="16"/>
       <c r="EY19" s="16"/>
@@ -13304,8 +13308,8 @@
       <c r="K20" s="33"/>
       <c r="L20" s="33"/>
       <c r="M20" s="18"/>
-      <c r="N20" s="18"/>
-      <c r="O20" s="18"/>
+      <c r="N20" s="33"/>
+      <c r="O20" s="33"/>
       <c r="P20" s="18"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="33"/>
@@ -13442,7 +13446,7 @@
       <c r="ES20" s="18"/>
       <c r="ET20" s="33"/>
       <c r="EU20" s="18"/>
-      <c r="EV20" s="18"/>
+      <c r="EV20" s="33"/>
       <c r="EW20" s="18"/>
       <c r="EX20" s="18"/>
       <c r="EY20" s="18"/>

</xml_diff>